<commit_message>
📊 Actualización automática del dashboard
</commit_message>
<xml_diff>
--- a/Comentarios Campaña.xlsx
+++ b/Comentarios Campaña.xlsx
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
@@ -565,7 +565,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554460671951520529', 'createTime': 1758909958, 'createTimeISO': '2025-09-26T18:05:58.000Z', 'text': 'Vuelvan los originales porfa😭', 'diggCount': 202, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7499982161161585680', 'uniqueId': 'lcv.xox', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/598c6e494574f43d995207087f02276a~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=23bc3af5&amp;x-expires=1759593600&amp;x-signature=oDHQ0OxhLNtcsBVbusbc2yYbm30%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554460671951520529', 'createTime': 1758909958, 'createTimeISO': '2025-09-26T18:05:58.000Z', 'text': 'Vuelvan los originales porfa😭', 'diggCount': 255, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7499982161161585680', 'uniqueId': 'lcv.xox', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/598c6e494574f43d995207087f02276a~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=2a53e9f8&amp;x-expires=1760619600&amp;x-signature=cO6vGikRyGRT4GJH4QZF1%2BcPSwA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -591,25 +591,25 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>saquen mochis en forma de looney toons 😁</t>
+          <t>y si soy de Colombia acá no hay Oxxo😭</t>
         </is>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45929.73829861111</v>
+        <v>45927.01857638889</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>45929</v>
+        <v>45927</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>17:43:09</t>
+          <t>00:26:45</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>189</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="L3" t="b">
         <v>0</v>
@@ -621,7 +621,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555568041485681424', 'createTime': 1759167789, 'createTimeISO': '2025-09-29T17:43:09.000Z', 'text': 'saquen mochis en forma de looney toons 😁', 'diggCount': 2, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6826404277322974214', 'uniqueId': 'carolinapr145', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/01f5729aadb40e0a6938515cce68a8d9~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=fb81a883&amp;x-expires=1759593600&amp;x-signature=gFwOxDt%2FNJNg%2F3YoE4EzQy0uIxQ%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554558807096722184', 'createTime': 1758932805, 'createTimeISO': '2025-09-27T00:26:45.000Z', 'text': 'y si soy de Colombia acá no hay Oxxo😭', 'diggCount': 189, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 62, 'uid': '7539632392610726919', 'uniqueId': 'samu07354', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/62b7de782c00747584315652ae6d84c0~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=7b13ac86&amp;x-expires=1760619600&amp;x-signature=gFvTr6hzjm3B7oX3mYldMgCEeAA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -647,25 +647,25 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>y si soy de Colombia acá no hay Oxxo😭</t>
+          <t>yo con mis 14 mochisaurios: 👁️👄👁</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>45927.01857638889</v>
+        <v>45943.24204861111</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>45927</v>
+        <v>45943</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>00:26:45</t>
+          <t>05:48:33</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="L4" t="b">
         <v>0</v>
@@ -677,7 +677,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554558807096722184', 'createTime': 1758932805, 'createTimeISO': '2025-09-27T00:26:45.000Z', 'text': 'y si soy de Colombia acá no hay Oxxo😭', 'diggCount': 120, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 39, 'uid': '7539632392610726919', 'uniqueId': 'samu07354', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/62b7de782c00747584315652ae6d84c0~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=efffe56d&amp;x-expires=1759593600&amp;x-signature=MdErwAfBBwUuIE3A0vg2U90b3Lk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7560579124269777672', 'createTime': 1760334513, 'createTimeISO': '2025-10-13T05:48:33.000Z', 'text': 'yo con mis 14 mochisaurios: 👁️👄👁', 'diggCount': 2, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7535556501164065799', 'uniqueId': 'flutershy46', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/5e5abe1cd68cf25fc519fc9b297b0c48~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=705f4834&amp;x-expires=1760619600&amp;x-signature=hSM6WLrtP6U1JJvqwxll6LlsjZs%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -703,25 +703,25 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Paso 1 compran un yogo yogo premio de tarrito y ya viene uno dentro.</t>
+          <t>mucho trabajo para un muñeco</t>
         </is>
       </c>
       <c r="G5" s="2" t="n">
-        <v>45932.67648148148</v>
+        <v>45928.12261574074</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>45932</v>
+        <v>45928</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>16:14:08</t>
+          <t>02:56:34</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>178</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L5" t="b">
         <v>0</v>
@@ -733,7 +733,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556658397476963090', 'createTime': 1759421648, 'createTimeISO': '2025-10-02T16:14:08.000Z', 'text': 'Paso 1 compran un yogo yogo premio de tarrito y ya viene uno dentro.', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7070376833845543941', 'uniqueId': 'yohanrojas85', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/0dc2488051a97fe07b1ff4157648948c~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=4fafc5ae&amp;x-expires=1759593600&amp;x-signature=8DcXmhxjxzxz5D2NCeQjJ9c94ek%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554968530820268818', 'createTime': 1759028194, 'createTimeISO': '2025-09-28T02:56:34.000Z', 'text': 'mucho trabajo para un muñeco', 'diggCount': 178, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 8, 'uid': '6900093665232208898', 'uniqueId': 'alonsocastaeda4', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/656e080d9831aeebef39b67358dbf496~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=a766fb9a&amp;x-expires=1760619600&amp;x-signature=8G%2FEU3VEKd1u9Sy8r6E9NBUdU6g%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -759,25 +759,25 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>pero están en todos los países ?</t>
+          <t>muy lindos pero huelen horrible🥺</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
-        <v>45926.73320601852</v>
+        <v>45934.07570601852</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>45926</v>
+        <v>45934</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>17:35:49</t>
+          <t>01:49:01</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L6" t="b">
         <v>0</v>
@@ -789,7 +789,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554452916247216913', 'createTime': 1758908149, 'createTimeISO': '2025-09-26T17:35:49.000Z', 'text': 'pero están en todos los países ?', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 2, 'uid': '7531534159044887568', 'uniqueId': 'nicolevargas2545', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/b5f68ad1a85740ea080fbebad18c2fbd~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=b9b3cb5b&amp;x-expires=1759593600&amp;x-signature=2IeS3kUwinITAOyUB2OQ%2F%2BHddvk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7557177612487262984', 'createTime': 1759542541, 'createTimeISO': '2025-10-04T01:49:01.000Z', 'text': 'muy lindos pero huelen horrible🥺', 'diggCount': 3, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7306290978125005830', 'uniqueId': 'tinta.prpura', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/325aa1206343248d1f45735372a84c0b~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=2ae1cb69&amp;x-expires=1760619600&amp;x-signature=lkg1639gdPlhe6x4G6HNNSmRI34%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -815,25 +815,25 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>los originales plissss</t>
+          <t>Mas fácil conseguirlos en el yogo premio</t>
         </is>
       </c>
       <c r="G7" s="2" t="n">
-        <v>45929.86050925926</v>
+        <v>45927.99311342592</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>45929</v>
+        <v>45927</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>20:39:08</t>
+          <t>23:50:05</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L7" t="b">
         <v>0</v>
@@ -845,7 +845,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555613367218963217', 'createTime': 1759178348, 'createTimeISO': '2025-09-29T20:39:08.000Z', 'text': 'los originales plissss', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7394864626544559109', 'uniqueId': 'user67670860120347', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/c0de0e4bb0938ad83a79077f7f67770d~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=287bb97f&amp;x-expires=1759593600&amp;x-signature=8BluVRzHyw1y4ZlNRBvbGESSg9s%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554920371642204949', 'createTime': 1759017005, 'createTimeISO': '2025-09-27T23:50:05.000Z', 'text': 'Mas fácil conseguirlos en el yogo premio', 'diggCount': 38, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 2, 'uid': '6517042462509241359', 'uniqueId': 'milenar96', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/65a89a7d9be3781e3c799109d941b1d0~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=e2a554a2&amp;x-expires=1760619600&amp;x-signature=wPsBBL4hf8xYatZYjduPth3qD4M%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -871,22 +871,22 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Alpina me mandan la caja Porfavor y les subo un video abriéndola</t>
+          <t>que triste que ya no salga las verdaderas figuritas de antes como lo era los Dioses del olimpo o los del futuro y los de goku y los futbolistas y los transformers y muchos mas, lo de hoy en dia ya me da pereza coleccionar esas cosas tan aburridas</t>
         </is>
       </c>
       <c r="G8" s="2" t="n">
-        <v>45931.93680555555</v>
+        <v>45945.17697916667</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>45931</v>
+        <v>45945</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>22:29:00</t>
+          <t>04:14:51</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -901,7 +901,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556383835371717396', 'createTime': 1759357740, 'createTimeISO': '2025-10-01T22:29:00.000Z', 'text': 'Alpina me mandan la caja Porfavor y les subo un video abriéndola', 'diggCount': 2, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7452119185666720773', 'uniqueId': 'juanjose192592', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/4cd1c36ecc1e938a7fbeb49be5a0bb2d~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=2891cc67&amp;x-expires=1759593600&amp;x-signature=rqch48b1JEiazidtz4MbUteSg60%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7561297143858135816', 'createTime': 1760501691, 'createTimeISO': '2025-10-15T04:14:51.000Z', 'text': 'que triste que ya no salga las verdaderas figuritas de antes como lo era los Dioses del olimpo o los del futuro y los de goku y los futbolistas y los transformers y muchos mas, lo de hoy en dia ya me da pereza coleccionar esas cosas tan aburridas', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7530133168200975368', 'uniqueId': 'figuritas07', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/musically-maliva-obj/1594805258216454~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=24e7ff38&amp;x-expires=1760619600&amp;x-signature=XcSDitOFZeEIWYaP6SnNYkRGn58%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -927,22 +927,22 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>en San Andrés no hay oxxo</t>
+          <t>saquen mochis en forma de looney toons 😁</t>
         </is>
       </c>
       <c r="G9" s="2" t="n">
-        <v>45933.62440972222</v>
+        <v>45929.73829861111</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>45933</v>
+        <v>45929</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>14:59:09</t>
+          <t>17:43:09</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -957,7 +957,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7557010184049443602', 'createTime': 1759503549, 'createTimeISO': '2025-10-03T14:59:09.000Z', 'text': 'en San Andrés no hay oxxo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7521449685388248071', 'uniqueId': 'lili0202028', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/dd40d81546424fd2fcea2ed3358909ad~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=088e250d&amp;x-expires=1759593600&amp;x-signature=GkzD4mK1MwLyBCxGHe0U16hVPBc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555568041485681424', 'createTime': 1759167789, 'createTimeISO': '2025-09-29T17:43:09.000Z', 'text': 'saquen mochis en forma de looney toons 😁', 'diggCount': 2, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6826404277322974214', 'uniqueId': 'carolinapr145', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/01f5729aadb40e0a6938515cce68a8d9~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=4b0faafd&amp;x-expires=1760619600&amp;x-signature=EMlrXv7omx9HsYYm2JfyaVFOP4Q%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -983,25 +983,25 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>en Colombia no hay OXXO</t>
+          <t>Alpina me mandan la caja Porfavor y les subo un video abriéndola</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
-        <v>45928.81866898148</v>
+        <v>45931.93680555555</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>45928</v>
+        <v>45931</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>19:38:53</t>
+          <t>22:29:00</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L10" t="b">
         <v>0</v>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555226815825003282', 'createTime': 1759088333, 'createTimeISO': '2025-09-28T19:38:53.000Z', 'text': 'en Colombia no hay OXXO', 'diggCount': 5, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 6, 'uid': '7239017294855767045', 'uniqueId': 'basspublicidadymediossas', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/27521fedb51ceea61f70eec021541ed1~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=97ac5676&amp;x-expires=1759593600&amp;x-signature=E4%2FFa%2BErgF%2BxC7BIYhE2bFZA4MI%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556383835371717396', 'createTime': 1759357740, 'createTimeISO': '2025-10-01T22:29:00.000Z', 'text': 'Alpina me mandan la caja Porfavor y les subo un video abriéndola', 'diggCount': 2, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7452119185666720773', 'uniqueId': 'juanjose192592', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/4cd1c36ecc1e938a7fbeb49be5a0bb2d~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=df4b8a7d&amp;x-expires=1760619600&amp;x-signature=YN6SjtIkM5wzdkSTDl5z7dzxGac%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1039,25 +1039,25 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>mucho trabajo para un muñeco</t>
+          <t>Una pregunta yo fui y lleve todas los logos de yogurt de vasito y me dijeron que esos no se ponían?</t>
         </is>
       </c>
       <c r="G11" s="2" t="n">
-        <v>45928.12261574074</v>
+        <v>45940.24515046296</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>45928</v>
+        <v>45940</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>02:56:34</t>
+          <t>05:53:01</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L11" t="b">
         <v>0</v>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554968530820268818', 'createTime': 1759028194, 'createTimeISO': '2025-09-28T02:56:34.000Z', 'text': 'mucho trabajo para un muñeco', 'diggCount': 65, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 5, 'uid': '6900093665232208898', 'uniqueId': 'alonsocastaeda4', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/656e080d9831aeebef39b67358dbf496~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=fe9ef00d&amp;x-expires=1759593600&amp;x-signature=Kdt%2FMlWSwRKxhW0IhduTyT0MmBo%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7559467019110204168', 'createTime': 1760075581, 'createTimeISO': '2025-10-10T05:53:01.000Z', 'text': 'Una pregunta yo fui y lleve todas los logos de yogurt de vasito y me dijeron que esos no se ponían?', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7546710335559959559', 'uniqueId': 'alexandrapardocaj', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/8cec9d771e97df3f8fa5b79f45eb0965~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=6a278b7e&amp;x-expires=1760619600&amp;x-signature=A73aV%2B7sePfhmb3pjVZwrjA09go%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1095,25 +1095,25 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ya we déjenlo pasar🥀</t>
+          <t>en Colombia no hay OXXO</t>
         </is>
       </c>
       <c r="G12" s="2" t="n">
-        <v>45928.95833333334</v>
+        <v>45928.81866898148</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>45928</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>23:00:00</t>
+          <t>19:38:53</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L12" t="b">
         <v>0</v>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555278564566205204', 'createTime': 1759100400, 'createTimeISO': '2025-09-28T23:00:00.000Z', 'text': 'ya we déjenlo pasar🥀', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7442938390251717687', 'uniqueId': 'solicituddeempleo0', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/778e7bf52d21ffd041c8cf4f95bc31e4~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=6e15c38c&amp;x-expires=1759593600&amp;x-signature=7%2BUMyanpyLNnRZdIxQBchKBALlc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555226815825003282', 'createTime': 1759088333, 'createTimeISO': '2025-09-28T19:38:53.000Z', 'text': 'en Colombia no hay OXXO', 'diggCount': 5, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 10, 'uid': '7239017294855767045', 'uniqueId': 'basspublicidadymediossas', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/27521fedb51ceea61f70eec021541ed1~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=df755315&amp;x-expires=1760619600&amp;x-signature=8yoSk2uAqJ%2BUysTAf7ttqusjD%2BY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1151,18 +1151,18 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>es mejor la paleta Drácula</t>
+          <t>nesecitoo la lista de los cuarenta muchis y nombrees</t>
         </is>
       </c>
       <c r="G13" s="2" t="n">
-        <v>45929.09761574074</v>
+        <v>45929.73436342592</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>45929</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>02:20:34</t>
+          <t>17:37:29</t>
         </is>
       </c>
       <c r="J13" t="n">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555330316220629781', 'createTime': 1759112434, 'createTimeISO': '2025-09-29T02:20:34.000Z', 'text': 'es mejor la paleta Drácula', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7470243338898408456', 'uniqueId': 'schneidermurchz', 'avatarThumbnail': 'https://p19-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/6def76385b3a465895b9c63a18974e36~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=594ab2c4&amp;x-expires=1759593600&amp;x-signature=9XjLmO6YdFbHHj9j1AEC4WId8x0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555566632794702599', 'createTime': 1759167449, 'createTimeISO': '2025-09-29T17:37:29.000Z', 'text': 'nesecitoo la lista de los cuarenta muchis y nombrees', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7476832145886741524', 'uniqueId': 'eli491676', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/de51a904dddc57525965d4639f48e5d4~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=529d76aa&amp;x-expires=1760619600&amp;x-signature=Bwf%2FNfTHwIZpo1hiyqJyjUfSSKY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1207,22 +1207,22 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>nena voy mal con la paleta Drácula y ya me pides que complete la de Mochis 🤣🤣</t>
+          <t>Que pereza tan vuelta!! y aquí estamos en Colombia porque una tienda de otra parte que no tiene presencia en toda Colombia.</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
-        <v>45930.3165625</v>
+        <v>45927.66452546296</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>45930</v>
+        <v>45927</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>07:35:51</t>
+          <t>15:56:55</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555782650826031873', 'createTime': 1759217751, 'createTimeISO': '2025-09-30T07:35:51.000Z', 'text': 'nena voy mal con la paleta Drácula y ya me pides que complete la de Mochis 🤣🤣', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6944546725642798085', 'uniqueId': 'juanluna5778', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/37c22dadb60b0803d8feaf140ff63274~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=fcabe48f&amp;x-expires=1759593600&amp;x-signature=GCd2O46sbQgJShvfiMEcKHx4uy0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554798543229666055', 'createTime': 1758988615, 'createTimeISO': '2025-09-27T15:56:55.000Z', 'text': 'Que pereza tan vuelta!! y aquí estamos en Colombia porque una tienda de otra parte que no tiene presencia en toda Colombia.', 'diggCount': 10, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7054390199678141445', 'uniqueId': 'monicakairos', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/00af4b97638212b23062f8a0c25de5cc~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=3eb1a4c7&amp;x-expires=1760619600&amp;x-signature=fDSePp2rs0BHA5vgq3hGIilGHEo%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1263,22 +1263,22 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>pasa lo mismo que con los Mochis anteriores va uno a reclamar y que no hay</t>
+          <t>Los Amooo pero Uyy un montón de cosas para el recambio!</t>
         </is>
       </c>
       <c r="G15" s="2" t="n">
-        <v>45926.8086574074</v>
+        <v>45927.14011574074</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>45926</v>
+        <v>45927</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>19:24:28</t>
+          <t>03:21:46</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554480920402084629', 'createTime': 1758914668, 'createTimeISO': '2025-09-26T19:24:28.000Z', 'text': 'pasa lo mismo que con los Mochis anteriores va uno a reclamar y que no hay', 'diggCount': 3, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7051306038071723013', 'uniqueId': '0604tn56mz', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/fe694ef60fa664d93b3af32ef8266baf~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=4ce06ed6&amp;x-expires=1759593600&amp;x-signature=%2FuP0AXzlJdEq%2B%2FuzX%2BqYD7XgDUU%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554603916571640577', 'createTime': 1758943306, 'createTimeISO': '2025-09-27T03:21:46.000Z', 'text': 'Los Amooo pero Uyy un montón de cosas para el recambio!', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7496003126047851521', 'uniqueId': 'caroprietog', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/193fc58d2631016bab3ea768e8d11296~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=ba55ccfe&amp;x-expires=1760619600&amp;x-signature=vI%2BRCZZFHZwX8zDuYYCE7qD9rxU%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1319,22 +1319,22 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Que pereza tan vuelta!! y aquí estamos en Colombia porque una tienda de otra parte que no tiene presencia en toda Colombia.</t>
+          <t>los originales plissss</t>
         </is>
       </c>
       <c r="G16" s="2" t="n">
-        <v>45927.66452546296</v>
+        <v>45929.86050925926</v>
       </c>
       <c r="H16" s="3" t="n">
-        <v>45927</v>
+        <v>45929</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>15:56:55</t>
+          <t>20:39:08</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554798543229666055', 'createTime': 1758988615, 'createTimeISO': '2025-09-27T15:56:55.000Z', 'text': 'Que pereza tan vuelta!! y aquí estamos en Colombia porque una tienda de otra parte que no tiene presencia en toda Colombia.', 'diggCount': 6, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7054390199678141445', 'uniqueId': 'monicakairos', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/00af4b97638212b23062f8a0c25de5cc~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=b54882f2&amp;x-expires=1759593600&amp;x-signature=cZP8fAylHazyFXhmkf%2Bs%2BrK8Pqo%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555613367218963217', 'createTime': 1759178348, 'createTimeISO': '2025-09-29T20:39:08.000Z', 'text': 'los originales plissss', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7394864626544559109', 'uniqueId': 'user67670860120347', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/c0de0e4bb0938ad83a79077f7f67770d~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=fcf0593f&amp;x-expires=1760619600&amp;x-signature=4jbzzCwlVbifjPW2j6osJRc6sv4%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1375,25 +1375,25 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>y si tengo repetidos no me los cambian 😂😂</t>
+          <t>pero están en todos los países ?</t>
         </is>
       </c>
       <c r="G17" s="2" t="n">
-        <v>45926.88744212963</v>
+        <v>45926.73320601852</v>
       </c>
       <c r="H17" s="3" t="n">
         <v>45926</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>21:17:55</t>
+          <t>17:35:49</t>
         </is>
       </c>
       <c r="J17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L17" t="b">
         <v>0</v>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554510104642650896', 'createTime': 1758921475, 'createTimeISO': '2025-09-26T21:17:55.000Z', 'text': 'y si tengo repetidos no me los cambian 😂😂', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6835450069409514502', 'uniqueId': 'ailatanollirum', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/474f3a22808ad684a516e4b07cab2a37~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=68854907&amp;x-expires=1759593600&amp;x-signature=%2BKldojfQKQy2E7gCKFKZz0xjWig%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554452916247216913', 'createTime': 1758908149, 'createTimeISO': '2025-09-26T17:35:49.000Z', 'text': 'pero están en todos los países ?', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 2, 'uid': '7531534159044887568', 'uniqueId': 'nicolevargas2545', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/b5f68ad1a85740ea080fbebad18c2fbd~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=fa741d76&amp;x-expires=1760619600&amp;x-signature=46Fvyg%2F2esJieGafpx7ZBE3nV4Y%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1431,25 +1431,25 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Mas fácil conseguirlos en el yogo premio</t>
+          <t>en Montería no hay OXXO pero si un todo a 1000 hay los entran</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
-        <v>45927.99311342592</v>
+        <v>45939.0350925926</v>
       </c>
       <c r="H18" s="3" t="n">
-        <v>45927</v>
+        <v>45939</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>23:50:05</t>
+          <t>00:50:32</t>
         </is>
       </c>
       <c r="J18" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L18" t="b">
         <v>0</v>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554920371642204949', 'createTime': 1759017005, 'createTimeISO': '2025-09-27T23:50:05.000Z', 'text': 'Mas fácil conseguirlos en el yogo premio', 'diggCount': 23, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 2, 'uid': '6517042462509241359', 'uniqueId': 'milenar96', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/65a89a7d9be3781e3c799109d941b1d0~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=5478023f&amp;x-expires=1759593600&amp;x-signature=4q63AXeCJAejdeCWqigZBUkEz9I%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7559017957411767047', 'createTime': 1759971032, 'createTimeISO': '2025-10-09T00:50:32.000Z', 'text': 'en Montería no hay OXXO pero si un todo a 1000 hay los entran', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7547836898510832661', 'uniqueId': 'liss05695', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/72682b59d508342205ec99b1085f60fa~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=b3362ad2&amp;x-expires=1760619600&amp;x-signature=kNb9V8fvrFxgnHj2pTkyeb2snd8%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1487,25 +1487,25 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>tengo un montón de Mochis de la primera colección, valdrá mucho?</t>
+          <t>y si no hay en mi ciudad Oxxo?</t>
         </is>
       </c>
       <c r="G19" s="2" t="n">
-        <v>45926.67013888889</v>
+        <v>45926.70601851852</v>
       </c>
       <c r="H19" s="3" t="n">
         <v>45926</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>16:05:00</t>
+          <t>16:56:40</t>
         </is>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L19" t="b">
         <v>0</v>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554429537663386376', 'createTime': 1758902700, 'createTimeISO': '2025-09-26T16:05:00.000Z', 'text': 'tengo un montón de Mochis de la primera colección, valdrá mucho?', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7116292147141166086', 'uniqueId': 'trades_fenix', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/9270efdc513746d459737e05d9dccbee~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=bbc3cf6d&amp;x-expires=1759593600&amp;x-signature=fTEnjFdeXObf%2F%2BnFzHn1Kv0KVCc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554442837019116305', 'createTime': 1758905800, 'createTimeISO': '2025-09-26T16:56:40.000Z', 'text': 'y si no hay en mi ciudad Oxxo?', 'diggCount': 11, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 3, 'uid': '7051817529568986117', 'uniqueId': 'mariana_priv.cs', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/7255c70c6e94d569e6bdbbdf98f98049~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=fd727aa2&amp;x-expires=1760619600&amp;x-signature=djSd9pPG21fgmu1LzrQV%2BueTvPk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1543,22 +1543,22 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>de cuánto se pueden reclamar</t>
+          <t>Paso 1 compran un yogo yogo premio de tarrito y ya viene uno dentro.</t>
         </is>
       </c>
       <c r="G20" s="2" t="n">
-        <v>45927.0343287037</v>
+        <v>45932.67648148148</v>
       </c>
       <c r="H20" s="3" t="n">
-        <v>45927</v>
+        <v>45932</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>00:49:26</t>
+          <t>16:14:08</t>
         </is>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554564660893696776', 'createTime': 1758934166, 'createTimeISO': '2025-09-27T00:49:26.000Z', 'text': 'de cuánto se pueden reclamar', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7197504067588178949', 'uniqueId': 'angelina.rodrguez432', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/7309230945578516485~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=366665d5&amp;x-expires=1759593600&amp;x-signature=luxQYiidg5iafdEty2Fyl7QWP0s%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556658397476963090', 'createTime': 1759421648, 'createTimeISO': '2025-10-02T16:14:08.000Z', 'text': 'Paso 1 compran un yogo yogo premio de tarrito y ya viene uno dentro.', 'diggCount': 2, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7070376833845543941', 'uniqueId': 'yohanrojas85', 'avatarThumbnail': 'https://p19-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/0dc2488051a97fe07b1ff4157648948c~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=74fdd8d5&amp;x-expires=1760619600&amp;x-signature=5vRdluKrTJs2xug2LFp1KqRdhjQ%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1599,25 +1599,25 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>y si no hay en mi ciudad Oxxo?</t>
+          <t>nena voy mal con la paleta Drácula y ya me pides que complete la de Mochis 🤣🤣</t>
         </is>
       </c>
       <c r="G21" s="2" t="n">
-        <v>45926.70601851852</v>
+        <v>45930.3165625</v>
       </c>
       <c r="H21" s="3" t="n">
-        <v>45926</v>
+        <v>45930</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>16:56:40</t>
+          <t>07:35:51</t>
         </is>
       </c>
       <c r="J21" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L21" t="b">
         <v>0</v>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554442837019116305', 'createTime': 1758905800, 'createTimeISO': '2025-09-26T16:56:40.000Z', 'text': 'y si no hay en mi ciudad Oxxo?', 'diggCount': 10, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 3, 'uid': '7051817529568986117', 'uniqueId': 'mariana_priv.cs', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/7255c70c6e94d569e6bdbbdf98f98049~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=34fae1cc&amp;x-expires=1759593600&amp;x-signature=SNT%2BVEwDwv26qDGGBzyPkefhpKc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555782650826031873', 'createTime': 1759217751, 'createTimeISO': '2025-09-30T07:35:51.000Z', 'text': 'nena voy mal con la paleta Drácula y ya me pides que complete la de Mochis 🤣🤣', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6944546725642798085', 'uniqueId': 'juanluna5778', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/37c22dadb60b0803d8feaf140ff63274~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=77fe576d&amp;x-expires=1760619600&amp;x-signature=oc04DXNk4%2FjsfBHpCl4dxt8DHQI%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1655,25 +1655,25 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>y si ya corte los logos y no dice mochi saurios y ya vote el empaque con el qr</t>
+          <t>Tanta cosa para uno</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
-        <v>45927.05542824074</v>
+        <v>45929.00190972222</v>
       </c>
       <c r="H22" s="3" t="n">
-        <v>45927</v>
+        <v>45929</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>01:19:49</t>
+          <t>00:02:45</t>
         </is>
       </c>
       <c r="J22" t="n">
         <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" t="b">
         <v>0</v>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554572506653803272', 'createTime': 1758935989, 'createTimeISO': '2025-09-27T01:19:49.000Z', 'text': 'y si ya corte los logos y no dice mochi saurios y ya vote el empaque con el qr', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '6887020420505109509', 'uniqueId': 'mari_a0131', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/52b610568365088bb8157c0e968fb5e0~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=ee5f368a&amp;x-expires=1759593600&amp;x-signature=XEgGeN9RITIpTX%2BwiIUeHw0u2GA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555294742864954119', 'createTime': 1759104165, 'createTimeISO': '2025-09-29T00:02:45.000Z', 'text': 'Tanta cosa para uno', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7243912158169465862', 'uniqueId': 'aguiilarpaolita', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/28050a045b8ba65347a8d82eb886b7be~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=61160427&amp;x-expires=1760619600&amp;x-signature=3s2CzClHdcTcIZRqbqmEbNDoXoc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1711,25 +1711,25 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>saquen ya otra colección 😕</t>
+          <t>pasa lo mismo que con los Mochis anteriores va uno a reclamar y que no hay</t>
         </is>
       </c>
       <c r="G23" s="2" t="n">
-        <v>45926.96346064815</v>
+        <v>45926.8086574074</v>
       </c>
       <c r="H23" s="3" t="n">
         <v>45926</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>23:07:23</t>
+          <t>19:24:28</t>
         </is>
       </c>
       <c r="J23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K23" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L23" t="b">
         <v>0</v>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554538366990189319', 'createTime': 1758928043, 'createTimeISO': '2025-09-26T23:07:23.000Z', 'text': 'saquen ya otra colección 😕', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 6, 'uid': '7430556660474758150', 'uniqueId': 'esobrad_1', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/496be0dadae6d46720222260f6036998~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=12f47ba7&amp;x-expires=1759593600&amp;x-signature=JL%2Fr%2BsBzcpFekBVMcYSvefonIlE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554480920402084629', 'createTime': 1758914668, 'createTimeISO': '2025-09-26T19:24:28.000Z', 'text': 'pasa lo mismo que con los Mochis anteriores va uno a reclamar y que no hay', 'diggCount': 3, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7051306038071723013', 'uniqueId': '0604tn56mz', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/fe694ef60fa664d93b3af32ef8266baf~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=d0f8cedf&amp;x-expires=1760619600&amp;x-signature=RAIlD%2B4TMgI2xVr4BaoQ5Mg7SOI%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1767,18 +1767,18 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>yo lo consigo en una papelera sin comprar el yogur</t>
+          <t>Soy de Colombia y vivo alado de un oxxo!! Yeii qué bien 😭💓💓</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
-        <v>45930.02420138889</v>
+        <v>45928.69695601852</v>
       </c>
       <c r="H24" s="3" t="n">
-        <v>45930</v>
+        <v>45928</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>00:34:51</t>
+          <t>16:43:37</t>
         </is>
       </c>
       <c r="J24" t="n">
@@ -1797,7 +1797,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555674134270001927', 'createTime': 1759192491, 'createTimeISO': '2025-09-30T00:34:51.000Z', 'text': 'yo lo consigo en una papelera sin comprar el yogur', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7384092541786014725', 'uniqueId': 'estrellita_alien', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/e38c298456b8a03417d891b1539c5b57~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=42a59fd2&amp;x-expires=1759593600&amp;x-signature=%2BoPyosacdc8ERTPJgLp1r5GOWEA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555181660511683346', 'createTime': 1759077817, 'createTimeISO': '2025-09-28T16:43:37.000Z', 'text': 'Soy de Colombia y vivo alado de un oxxo!! Yeii qué bien 😭💓💓', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7468722166260876295', 'uniqueId': 'honey.mimi7', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/b82704ac6df483016e5b03a909c6379e~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=2f6d7b48&amp;x-expires=1760619600&amp;x-signature=kMP3CWMv%2BXHmjmG4P6l7ofZ1EJk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1823,22 +1823,22 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>pero si no tengo un OXXO cerca 😃</t>
+          <t>ya we déjenlo pasar🥀</t>
         </is>
       </c>
       <c r="G25" s="2" t="n">
-        <v>45926.88136574074</v>
+        <v>45928.95833333334</v>
       </c>
       <c r="H25" s="3" t="n">
-        <v>45926</v>
+        <v>45928</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>21:09:10</t>
+          <t>23:00:00</t>
         </is>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" t="n">
         <v>0</v>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554507901999022866', 'createTime': 1758920950, 'createTimeISO': '2025-09-26T21:09:10.000Z', 'text': 'pero si no tengo un OXXO cerca 😃', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7541548984452891666', 'uniqueId': 'jesu_7146', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/d4e69f45d9727cf6af8705941b8c64ea~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=e8f13fa6&amp;x-expires=1759593600&amp;x-signature=s4dV%2FhFeeYOj4qBAE7CJHxKyENw%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555278564566205204', 'createTime': 1759100400, 'createTimeISO': '2025-09-28T23:00:00.000Z', 'text': 'ya we déjenlo pasar🥀', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7442938390251717687', 'uniqueId': 'solicituddeempleo0', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/778e7bf52d21ffd041c8cf4f95bc31e4~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=65bd0805&amp;x-expires=1760619600&amp;x-signature=e0An34XRXmZZjF%2FrpNSc6mNULe0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1879,25 +1879,25 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Y si no hay Oxxo en la ciudad?</t>
+          <t>Mucha vaina pa eso</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
-        <v>45926.98476851852</v>
+        <v>45928.76012731482</v>
       </c>
       <c r="H26" s="3" t="n">
-        <v>45926</v>
+        <v>45928</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>23:38:04</t>
+          <t>18:14:35</t>
         </is>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" t="b">
         <v>0</v>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554546221059883796', 'createTime': 1758929884, 'createTimeISO': '2025-09-26T23:38:04.000Z', 'text': 'Y si no hay Oxxo en la ciudad?', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '6960146577365419014', 'uniqueId': 'sebas_20114', 'avatarThumbnail': 'https://p19-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/35fcab65e640a5b27c092124d8b2047e~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=6c5e656e&amp;x-expires=1759593600&amp;x-signature=%2FXoYwIsqMHp8z%2FljjuCCr6ZTnJA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555205113074369287', 'createTime': 1759083275, 'createTimeISO': '2025-09-28T18:14:35.000Z', 'text': 'Mucha vaina pa eso', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6936408559421850630', 'uniqueId': 'drea._.00', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/bcf053ea8caaedad5bd9faac784342b9~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=367a5692&amp;x-expires=1760619600&amp;x-signature=fwF33MZmgOo43M%2FBiKQ%2BenYcRTg%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1935,25 +1935,25 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Y si en Neiva no hay Oxxo 😐</t>
+          <t>es mejor la paleta Drácula</t>
         </is>
       </c>
       <c r="G27" s="2" t="n">
-        <v>45927.88842592593</v>
+        <v>45929.09761574074</v>
       </c>
       <c r="H27" s="3" t="n">
-        <v>45927</v>
+        <v>45929</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>21:19:20</t>
+          <t>02:20:34</t>
         </is>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" t="b">
         <v>0</v>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554881592553718535', 'createTime': 1759007960, 'createTimeISO': '2025-09-27T21:19:20.000Z', 'text': 'Y si en Neiva no hay Oxxo 😐', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7525546550606758919', 'uniqueId': 'julianavanegas312', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/7bbf565d8eb052ba174287777f6a6684~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=ffe5c33f&amp;x-expires=1759593600&amp;x-signature=f%2FviKegr02o4AWmfx4o1anNxT7I%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555330316220629781', 'createTime': 1759112434, 'createTimeISO': '2025-09-29T02:20:34.000Z', 'text': 'es mejor la paleta Drácula', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7470243338898408456', 'uniqueId': 'schneidermurchz', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/e38e7ec35870b748223e8cb22c6d237a~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=a00cacf9&amp;x-expires=1760619600&amp;x-signature=PANpEqFbA7g0FPKTfFY9GHwArUs%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -1991,25 +1991,25 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>yo los compré y cuando lo abrí me salió una pa pegar en el bolso</t>
+          <t>en Colombia no hay OXXO y venden los yogo premio muy caros ):</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
-        <v>45928.13539351852</v>
+        <v>45941.73184027777</v>
       </c>
       <c r="H28" s="3" t="n">
-        <v>45928</v>
+        <v>45941</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>03:14:58</t>
+          <t>17:33:51</t>
         </is>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28" t="b">
         <v>0</v>
@@ -2021,7 +2021,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554973274371982100', 'createTime': 1759029298, 'createTimeISO': '2025-09-28T03:14:58.000Z', 'text': 'yo los compré y cuando lo abrí me salió una pa pegar en el bolso', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7364179204911137798', 'uniqueId': 'zephyts_', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/c86a63fa4fb27a6057c14957a56b9a1d~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=4159aa22&amp;x-expires=1759593600&amp;x-signature=WlWWgzKbaOE2w1ArPcnU%2BXcXtmU%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7560018722665284360', 'createTime': 1760204031, 'createTimeISO': '2025-10-11T17:33:51.000Z', 'text': 'en Colombia no hay OXXO y venden los yogo premio muy caros ):', 'diggCount': 2, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7517389511912424455', 'uniqueId': 'tokito_team_black', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/afa29d1e92a17252e840cfdca3edbe82~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=b827bf04&amp;x-expires=1760619600&amp;x-signature=w%2B8B6RKdulJJsuyVzZ6jIw6DIhg%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2047,22 +2047,22 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Yo el otro día compré uno de esos y los derretí para hacer uno mega.</t>
+          <t>de cuánto se pueden reclamar</t>
         </is>
       </c>
       <c r="G29" s="2" t="n">
-        <v>45927.61450231481</v>
+        <v>45927.0343287037</v>
       </c>
       <c r="H29" s="3" t="n">
         <v>45927</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>14:44:53</t>
+          <t>00:49:26</t>
         </is>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554779983777989383', 'createTime': 1758984293, 'createTimeISO': '2025-09-27T14:44:53.000Z', 'text': 'Yo el otro día compré uno de esos y los derretí para hacer uno mega.', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7390881053177955334', 'uniqueId': 'elpanamiguel7528', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/0dbaa0de347c3ac93474b7346f4d9ff6~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=1236a833&amp;x-expires=1759593600&amp;x-signature=5Ulql%2FlfyaVDnCK0VcybUf9aYuU%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554564660893696776', 'createTime': 1758934166, 'createTimeISO': '2025-09-27T00:49:26.000Z', 'text': 'de cuánto se pueden reclamar', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7197504067588178949', 'uniqueId': 'angelina.rodrguez432', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/7309230945578516485~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=ee59d39a&amp;x-expires=1760619600&amp;x-signature=%2Fo8nNsfV7ULP2NA9Y398O0%2F4rTY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2103,25 +2103,25 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Siempre me toca el mismo caracol amarillo 🥺</t>
+          <t>he ido al los OXXO que aparecen y nunca los dan dicen que no tiene idea de que se trata</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
-        <v>45929.96003472222</v>
+        <v>45934.87288194444</v>
       </c>
       <c r="H30" s="3" t="n">
-        <v>45929</v>
+        <v>45934</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>23:02:27</t>
+          <t>20:56:57</t>
         </is>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" t="b">
         <v>0</v>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555650338171339527', 'createTime': 1759186947, 'createTimeISO': '2025-09-29T23:02:27.000Z', 'text': 'Siempre me toca el mismo caracol amarillo 🥺', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7524391539830948872', 'uniqueId': 'nataliavall', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/4f090b395f31d1fc53fc8a1d40867af3~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=c3e56102&amp;x-expires=1759593600&amp;x-signature=7d%2BkJ3qQQ6bgTgoos3A1dYFNjXI%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7557473388605375233', 'createTime': 1759611417, 'createTimeISO': '2025-10-04T20:56:57.000Z', 'text': 'he ido al los OXXO que aparecen y nunca los dan dicen que no tiene idea de que se trata', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7216783190328181765', 'uniqueId': 'leocambell10', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/6010b651447b2c3934e2d7ede50948f0~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=b0ead81c&amp;x-expires=1760619600&amp;x-signature=24KqBsXeOTBYzFcvQ27VPIpkFf4%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2159,22 +2159,22 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>pero si ya corte los logos y no corte lo que dice mochisaurios y tampoco tengo el código??</t>
+          <t>todos los lugares no tiene esa tienda entonces para que hacen eso</t>
         </is>
       </c>
       <c r="G31" s="2" t="n">
-        <v>45929.11127314815</v>
+        <v>45929.98554398148</v>
       </c>
       <c r="H31" s="3" t="n">
         <v>45929</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>02:40:14</t>
+          <t>23:39:11</t>
         </is>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="n">
         <v>1</v>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555335413934981895', 'createTime': 1759113614, 'createTimeISO': '2025-09-29T02:40:14.000Z', 'text': 'pero si ya corte los logos y no corte lo que dice mochisaurios y tampoco tengo el código??', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '6887020420505109509', 'uniqueId': 'mari_a0131', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/52b610568365088bb8157c0e968fb5e0~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=ee5f368a&amp;x-expires=1759593600&amp;x-signature=XEgGeN9RITIpTX%2BwiIUeHw0u2GA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555659801544475400', 'createTime': 1759189151, 'createTimeISO': '2025-09-29T23:39:11.000Z', 'text': 'todos los lugares no tiene esa tienda entonces para que hacen eso', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '6817635812092937221', 'uniqueId': 'd.a.n.y.y.20', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/2de29fc766d1e8cb0e09c7aa6f907237~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=8587adca&amp;x-expires=1760619600&amp;x-signature=Jf94b0NnIZ0VUVPeGUu0wNIt72Y%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2215,25 +2215,26 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>todos los lugares no tiene esa tienda entonces para que hacen eso</t>
+          <t>me encantan estos mochis pero quisiera saber el nombre de 5
+los muñequitos 🥰</t>
         </is>
       </c>
       <c r="G32" s="2" t="n">
-        <v>45929.98554398148</v>
+        <v>45932.51024305556</v>
       </c>
       <c r="H32" s="3" t="n">
-        <v>45929</v>
+        <v>45932</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>23:39:11</t>
+          <t>12:14:45</t>
         </is>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L32" t="b">
         <v>0</v>
@@ -2245,7 +2246,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555659801544475400', 'createTime': 1759189151, 'createTimeISO': '2025-09-29T23:39:11.000Z', 'text': 'todos los lugares no tiene esa tienda entonces para que hacen eso', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '6817635812092937221', 'uniqueId': 'd.a.n.y.y.20', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/2de29fc766d1e8cb0e09c7aa6f907237~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=865f634d&amp;x-expires=1759593600&amp;x-signature=CXrFzHbvCgpOVlDIpghjuhKYrs0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556596683191681808', 'createTime': 1759407285, 'createTimeISO': '2025-10-02T12:14:45.000Z', 'text': 'me encantan estos mochis pero quisiera saber el nombre de 5\nlos muñequitos 🥰', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 2, 'uid': '6958943464231011333', 'uniqueId': 'jsa_4567', 'avatarThumbnail': 'https://p77-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/68932c07b5db5c7e5aba191de5535be2~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=f465fd1e&amp;x-expires=1760619600&amp;x-signature=etInJAJZp6%2F%2F2rm0URs%2BTToPxdg%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2271,18 +2272,18 @@
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>en todas las tiendas</t>
+          <t>Que yo sepa que en Colombia no ay oxoxo</t>
         </is>
       </c>
       <c r="G33" s="2" t="n">
-        <v>45929.71753472222</v>
+        <v>45935.77436342592</v>
       </c>
       <c r="H33" s="3" t="n">
-        <v>45929</v>
+        <v>45935</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>17:13:15</t>
+          <t>18:35:05</t>
         </is>
       </c>
       <c r="J33" t="n">
@@ -2301,7 +2302,7 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555560366673462037', 'createTime': 1759165995, 'createTimeISO': '2025-09-29T17:13:15.000Z', 'text': 'en todas las tiendas', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7285382001250141189', 'uniqueId': 'rosycastellanos86', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/7321737955369582597~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=83335183&amp;x-expires=1759593600&amp;x-signature=uh%2FvrCmVF2TkHmqmWuC%2B69C49fk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7557807940859937554', 'createTime': 1759689305, 'createTimeISO': '2025-10-05T18:35:05.000Z', 'text': 'Que yo sepa que en Colombia no ay oxoxo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7543462359529440276', 'uniqueId': 'annie.carolina7', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/d2456170bcdac850e36cf4089df9b648~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=ed5c0cb1&amp;x-expires=1760619600&amp;x-signature=ouVG3d%2Bufr0GGoAmeWdbW9Xm0iE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2327,25 +2328,25 @@
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>pero en mi ciudad no hay oxxo</t>
+          <t>yo ya tengo uno MUEJEJEJEJJE</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
-        <v>45926.83740740741</v>
+        <v>45943.88428240741</v>
       </c>
       <c r="H34" s="3" t="n">
-        <v>45926</v>
+        <v>45943</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>20:05:52</t>
+          <t>21:13:22</t>
         </is>
       </c>
       <c r="J34" t="n">
         <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L34" t="b">
         <v>0</v>
@@ -2357,7 +2358,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554491584386548498', 'createTime': 1758917152, 'createTimeISO': '2025-09-26T20:05:52.000Z', 'text': 'pero en mi ciudad no hay oxxo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7260695820469830662', 'uniqueId': 'sara.belen10', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/3d27eeec13984e1bfdd89a0226103589~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=48bc7712&amp;x-expires=1759593600&amp;x-signature=g2ShFs02LLhpkbR9QbEzP3qx3I8%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7560817334177645328', 'createTime': 1760390002, 'createTimeISO': '2025-10-13T21:13:22.000Z', 'text': 'yo ya tengo uno MUEJEJEJEJJE', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7531534159044887568', 'uniqueId': 'nicolevargas2545', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/b5f68ad1a85740ea080fbebad18c2fbd~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=77ddfe70&amp;x-expires=1760619600&amp;x-signature=P%2FrabsgEQvpMRxgyPGJ8rcpw1qo%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2383,26 +2384,25 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>me encantan estos mochis pero quisiera saber el nombre de 5
-los muñequitos 🥰</t>
+          <t>a poco hay OXXO en colombia</t>
         </is>
       </c>
       <c r="G35" s="2" t="n">
-        <v>45932.51024305556</v>
+        <v>45937.70814814815</v>
       </c>
       <c r="H35" s="3" t="n">
-        <v>45932</v>
+        <v>45937</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>12:14:45</t>
+          <t>16:59:44</t>
         </is>
       </c>
       <c r="J35" t="n">
         <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L35" t="b">
         <v>0</v>
@@ -2414,7 +2414,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556596683191681808', 'createTime': 1759407285, 'createTimeISO': '2025-10-02T12:14:45.000Z', 'text': 'me encantan estos mochis pero quisiera saber el nombre de 5\nlos muñequitos 🥰', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 2, 'uid': '6958943464231011333', 'uniqueId': 'jsa_4567', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/68932c07b5db5c7e5aba191de5535be2~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=5101edd0&amp;x-expires=1759593600&amp;x-signature=CSmOWWGwC3%2B0zazrSRw0h8OoLbI%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7558525593814467336', 'createTime': 1759856384, 'createTimeISO': '2025-10-07T16:59:44.000Z', 'text': 'a poco hay OXXO en colombia', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7300666454697362438', 'uniqueId': 'cristiancardona16', 'avatarThumbnail': 'https://p77-sign-va.tiktokcdn.com/tos-maliva-avt-0068/1169cb00c9709b98aa7a2c6299d6372c~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=3f03b978&amp;x-expires=1760619600&amp;x-signature=2NOhy3LHNjwrquQ4h1B1dAcG6HM%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2440,25 +2440,25 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>los dan todos</t>
+          <t>pero en mi ciudad no hay oxxo</t>
         </is>
       </c>
       <c r="G36" s="2" t="n">
-        <v>45932.8313425926</v>
+        <v>45926.83740740741</v>
       </c>
       <c r="H36" s="3" t="n">
-        <v>45932</v>
+        <v>45926</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>19:57:08</t>
+          <t>20:05:52</t>
         </is>
       </c>
       <c r="J36" t="n">
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" t="b">
         <v>0</v>
@@ -2470,7 +2470,7 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556715834195788562', 'createTime': 1759435028, 'createTimeISO': '2025-10-02T19:57:08.000Z', 'text': 'los dan todos', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7193838219199251461', 'uniqueId': 'emmanuel.monte', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/def659400c8d341d374792bc4c83b7a8~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=8efb5d60&amp;x-expires=1759593600&amp;x-signature=Z63nnfXVcaWFSYLl6tKJ3tDCvAo%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554491584386548498', 'createTime': 1758917152, 'createTimeISO': '2025-09-26T20:05:52.000Z', 'text': 'pero en mi ciudad no hay oxxo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7260695820469830662', 'uniqueId': 'sara.belen10', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/3d27eeec13984e1bfdd89a0226103589~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=618a330d&amp;x-expires=1760619600&amp;x-signature=CGM7EpncQE8tdcX8k7vHJTYK8pk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2496,18 +2496,18 @@
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>no hay en Neiva 😓</t>
+          <t>en todas las tiendas</t>
         </is>
       </c>
       <c r="G37" s="2" t="n">
-        <v>45929.74864583334</v>
+        <v>45929.71753472222</v>
       </c>
       <c r="H37" s="3" t="n">
         <v>45929</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>17:58:03</t>
+          <t>17:13:15</t>
         </is>
       </c>
       <c r="J37" t="n">
@@ -2526,7 +2526,7 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555571926753313544', 'createTime': 1759168683, 'createTimeISO': '2025-09-29T17:58:03.000Z', 'text': 'no hay en Neiva 😓', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7182010915348857861', 'uniqueId': 'jerzxz1', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/7fda5e90141d8eb3debf58517b07cfb3~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=08189add&amp;x-expires=1759593600&amp;x-signature=6yC%2FqGMtQ%2F7cPfkzNhCyrjXgLeI%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555560366673462037', 'createTime': 1759165995, 'createTimeISO': '2025-09-29T17:13:15.000Z', 'text': 'en todas las tiendas', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7285382001250141189', 'uniqueId': 'rosycastellanos86', 'avatarThumbnail': 'https://p77-sign-va.tiktokcdn.com/tos-maliva-avt-0068/7321737955369582597~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=14c7b6c5&amp;x-expires=1760619600&amp;x-signature=52lATCW8RPxyXtyejSevw8D6hJ0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2552,25 +2552,25 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Yo tengo el Oxxo a la esquina</t>
+          <t>Ya tengo 8</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
-        <v>45929.82648148148</v>
+        <v>45942.84155092593</v>
       </c>
       <c r="H38" s="3" t="n">
-        <v>45929</v>
+        <v>45942</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>19:50:08</t>
+          <t>20:11:50</t>
         </is>
       </c>
       <c r="J38" t="n">
         <v>0</v>
       </c>
       <c r="K38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L38" t="b">
         <v>0</v>
@@ -2582,7 +2582,7 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555600732201698064', 'createTime': 1759175408, 'createTimeISO': '2025-09-29T19:50:08.000Z', 'text': 'Yo tengo el Oxxo a la esquina', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '6998604116167656453', 'uniqueId': 'estrellita_7291', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/1f013694362e5b7acf25ef66d2a1224c~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=5fc0dd9e&amp;x-expires=1759593600&amp;x-signature=u72Yyqd4%2BV%2B0KvbGhQ%2BLrepyPaA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7560430479338930962', 'createTime': 1760299910, 'createTimeISO': '2025-10-12T20:11:50.000Z', 'text': 'Ya tengo 8', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7420101536925713413', 'uniqueId': 'creeper_705', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/b2e2db3ec04397fe9ef4b7153c635707~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=001c5b95&amp;x-expires=1760619600&amp;x-signature=BLDxEMcFlFlvLhae9zavoaVuKbU%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2608,18 +2608,18 @@
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>oiga mano lastima que todavía no salen los mochisaurios en los yogopremios</t>
+          <t>Y si en Neiva no hay Oxxo 😐</t>
         </is>
       </c>
       <c r="G39" s="2" t="n">
-        <v>45930.30774305556</v>
+        <v>45927.88842592593</v>
       </c>
       <c r="H39" s="3" t="n">
-        <v>45930</v>
+        <v>45927</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>07:23:09</t>
+          <t>21:19:20</t>
         </is>
       </c>
       <c r="J39" t="n">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555779391944016647', 'createTime': 1759216989, 'createTimeISO': '2025-09-30T07:23:09.000Z', 'text': 'oiga mano lastima que todavía no salen los mochisaurios en los yogopremios', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7112525176407737350', 'uniqueId': 'esteban_castillo.220', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/8331a286f4c2f1e0d41f74df6a541951~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=c122a87c&amp;x-expires=1759593600&amp;x-signature=lvAKmiShDXDnOYkVBBukoUtvKkE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554881592553718535', 'createTime': 1759007960, 'createTimeISO': '2025-09-27T21:19:20.000Z', 'text': 'Y si en Neiva no hay Oxxo 😐', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7525546550606758919', 'uniqueId': 'julianavanegas312', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/7bbf565d8eb052ba174287777f6a6684~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=35321f4b&amp;x-expires=1760619600&amp;x-signature=w72eyw74AU%2FR3tbHfKoaEL4Za94%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2664,25 +2664,25 @@
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Aquí en Cartagena no ha Oxxos 🥺🥺🥺</t>
+          <t>no me salió el mochi en el yogurt</t>
         </is>
       </c>
       <c r="G40" s="2" t="n">
-        <v>45927.68152777778</v>
+        <v>45944.93458333334</v>
       </c>
       <c r="H40" s="3" t="n">
-        <v>45927</v>
+        <v>45944</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>16:21:24</t>
+          <t>22:25:48</t>
         </is>
       </c>
       <c r="J40" t="n">
         <v>0</v>
       </c>
       <c r="K40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" t="b">
         <v>0</v>
@@ -2694,7 +2694,7 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554804848962847506', 'createTime': 1758990084, 'createTimeISO': '2025-09-27T16:21:24.000Z', 'text': 'Aquí en Cartagena no ha Oxxos 🥺🥺🥺', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '6737168611750626309', 'uniqueId': 'idangeral', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/3efcd03d865b92dfa9ffd78e82854da1~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=21ecf9c1&amp;x-expires=1759593600&amp;x-signature=DO%2BTNmAsxCQImYRBLVZiMhTo8VQ%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7561207129513509650', 'createTime': 1760480748, 'createTimeISO': '2025-10-14T22:25:48.000Z', 'text': 'no me salió el mochi en el yogurt', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7446973923780641797', 'uniqueId': 'storytime_de_terror18', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/3bf4c3dd2c2cd49f7beb82132f8bf73a~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=5cb60514&amp;x-expires=1760619600&amp;x-signature=0cW8eNhVeoNhBVieOzCMYBl8zcw%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2720,25 +2720,25 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>eso pa que</t>
+          <t>Aquí en Cartagena no ha Oxxos 🥺🥺🥺</t>
         </is>
       </c>
       <c r="G41" s="2" t="n">
-        <v>45928.22596064815</v>
+        <v>45927.68152777778</v>
       </c>
       <c r="H41" s="3" t="n">
-        <v>45928</v>
+        <v>45927</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>05:25:23</t>
+          <t>16:21:24</t>
         </is>
       </c>
       <c r="J41" t="n">
         <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" t="b">
         <v>0</v>
@@ -2750,7 +2750,7 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555006889290826503', 'createTime': 1759037123, 'createTimeISO': '2025-09-28T05:25:23.000Z', 'text': 'eso pa que', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7542870679370417160', 'uniqueId': 'x_xxx660', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/baad79b549774584b1a67ebfc08f5a67~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=a164f4bf&amp;x-expires=1759593600&amp;x-signature=mfUwT7ynHRct8asHaTUskhD4v%2BY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554804848962847506', 'createTime': 1758990084, 'createTimeISO': '2025-09-27T16:21:24.000Z', 'text': 'Aquí en Cartagena no ha Oxxos 🥺🥺🥺', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '6737168611750626309', 'uniqueId': 'idangeral', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/3efcd03d865b92dfa9ffd78e82854da1~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=89f6ef23&amp;x-expires=1760619600&amp;x-signature=pg7opzAPgGM0aX6RUIE3kMDY2HE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2776,25 +2776,25 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Clarion esq en todos los países hay OXXO 🌚🌝</t>
+          <t>oiga mano lastima que todavía no salen los mochisaurios en los yogopremios</t>
         </is>
       </c>
       <c r="G42" s="2" t="n">
-        <v>45932.87021990741</v>
+        <v>45930.30774305556</v>
       </c>
       <c r="H42" s="3" t="n">
-        <v>45932</v>
+        <v>45930</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>20:53:07</t>
+          <t>07:23:09</t>
         </is>
       </c>
       <c r="J42" t="n">
         <v>0</v>
       </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L42" t="b">
         <v>0</v>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556730178652275472', 'createTime': 1759438387, 'createTimeISO': '2025-10-02T20:53:07.000Z', 'text': 'Clarion esq en todos los países hay OXXO 🌚🌝', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7396657590753100805', 'uniqueId': 'ariadnna.muoz', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/9279bed9092f96fb07b2504a5c7ed70d~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=fa6bf3ca&amp;x-expires=1759593600&amp;x-signature=i9%2BebeGVvoDMH5qmYDkF6UPZUF4%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555779391944016647', 'createTime': 1759216989, 'createTimeISO': '2025-09-30T07:23:09.000Z', 'text': 'oiga mano lastima que todavía no salen los mochisaurios en los yogopremios', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 2, 'uid': '7112525176407737350', 'uniqueId': 'esteban_castillo.220', 'avatarThumbnail': 'https://p77-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/8331a286f4c2f1e0d41f74df6a541951~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=30f54cae&amp;x-expires=1760619600&amp;x-signature=%2Fdcuv1pf1SCqHDYVzuGGdhcZfuk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2832,18 +2832,18 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>me encantan</t>
+          <t>A QUIEN SIGOOOO❓ TEAM NEGRO[wicked]</t>
         </is>
       </c>
       <c r="G43" s="2" t="n">
-        <v>45932.03704861111</v>
+        <v>45934.12070601852</v>
       </c>
       <c r="H43" s="3" t="n">
-        <v>45932</v>
+        <v>45934</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>00:53:21</t>
+          <t>02:53:49</t>
         </is>
       </c>
       <c r="J43" t="n">
@@ -2862,7 +2862,7 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556421084930458375', 'createTime': 1759366401, 'createTimeISO': '2025-10-02T00:53:21.000Z', 'text': 'me encantan', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7321905632369361926', 'uniqueId': 'peluchero0', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/c3dcf3f4636b10f771ee500678138dfb~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=10e188d6&amp;x-expires=1759593600&amp;x-signature=LkYDF32WzE%2BUARMKqE6zRU%2BUMjE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7557194342633718546', 'createTime': 1759546429, 'createTimeISO': '2025-10-04T02:53:49.000Z', 'text': '𝘼 𝙌𝙐𝙄𝙀𝙉 𝙎𝙄𝙂𝙊𝙊𝙊𝙊❓ TEAM NEGRO[wicked]', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7428462608468853765', 'uniqueId': 'freestyle11.4', 'avatarThumbnail': 'https://p77-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/d77e4d9d34078046d77184cafe9499c3~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=6445304e&amp;x-expires=1760619600&amp;x-signature=aUuY9DcmD03bSU2UvHnAoDdfr24%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2888,18 +2888,18 @@
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>como</t>
+          <t>Pensé que crecían en el agua 😁😂</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
-        <v>45932.00744212963</v>
+        <v>45945.00143518519</v>
       </c>
       <c r="H44" s="3" t="n">
-        <v>45932</v>
+        <v>45945</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>00:10:43</t>
+          <t>00:02:04</t>
         </is>
       </c>
       <c r="J44" t="n">
@@ -2918,7 +2918,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556410076190638855', 'createTime': 1759363843, 'createTimeISO': '2025-10-02T00:10:43.000Z', 'text': 'como', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7529699467920409601', 'uniqueId': 'diego.chacon.ruiz', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/0ec5d98d45bb80659e129294e7556e6b~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=d810592c&amp;x-expires=1759593600&amp;x-signature=f4fgfjGEDai%2FcpJnu38tx2aCylc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7561231968739656466', 'createTime': 1760486524, 'createTimeISO': '2025-10-15T00:02:04.000Z', 'text': 'Pensé que crecían en el agua 😁😂', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7095002096173368325', 'uniqueId': 'camiloserna.8173', 'avatarThumbnail': 'https://p77-sign-va.tiktokcdn.com/tos-maliva-avt-0068/4f82b1d4beaab8b506d3f312e534a68f~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=0f78718a&amp;x-expires=1760619600&amp;x-signature=k0DDjoBao6HdCHi0EbWmWr5AECE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -2944,25 +2944,25 @@
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>part 2</t>
+          <t>no hay en Neiva 😓</t>
         </is>
       </c>
       <c r="G45" s="2" t="n">
-        <v>45929.57021990741</v>
+        <v>45929.74864583334</v>
       </c>
       <c r="H45" s="3" t="n">
         <v>45929</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>13:41:07</t>
+          <t>17:58:03</t>
         </is>
       </c>
       <c r="J45" t="n">
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L45" t="b">
         <v>0</v>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555505705790538514', 'createTime': 1759153267, 'createTimeISO': '2025-09-29T13:41:07.000Z', 'text': 'part 2', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7518189866266526728', 'uniqueId': 'jenny.loango', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/0aa7aaecbe34f7dd94d1887fac659dec~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=92d62253&amp;x-expires=1759593600&amp;x-signature=58p2PlUCCd%2B8B4%2BCLc6j4r6pZAs%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555571926753313544', 'createTime': 1759168683, 'createTimeISO': '2025-09-29T17:58:03.000Z', 'text': 'no hay en Neiva 😓', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7182010915348857861', 'uniqueId': 'jerzxz1', 'avatarThumbnail': 'https://p77-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/7fda5e90141d8eb3debf58517b07cfb3~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=1913fef9&amp;x-expires=1760619600&amp;x-signature=W8EkiAcgcoL3zZpkzfC2WKHeJfo%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3000,18 +3000,18 @@
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>amooo los mochiss</t>
+          <t>en colombia no ay oxxo</t>
         </is>
       </c>
       <c r="G46" s="2" t="n">
-        <v>45930.14606481481</v>
+        <v>45941.11943287037</v>
       </c>
       <c r="H46" s="3" t="n">
-        <v>45930</v>
+        <v>45941</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>03:30:20</t>
+          <t>02:51:59</t>
         </is>
       </c>
       <c r="J46" t="n">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555719396933829377', 'createTime': 1759203020, 'createTimeISO': '2025-09-30T03:30:20.000Z', 'text': 'amooo los mochiss', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7367208908349621253', 'uniqueId': 'temasammy', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/653ff6c74910183d0e2794469e78393f~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=c9d23517&amp;x-expires=1759593600&amp;x-signature=UrdndgdkaCwRIktGRyAF0PFnVTA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7559791437481788178', 'createTime': 1760151119, 'createTimeISO': '2025-10-11T02:51:59.000Z', 'text': 'en colombia no ay oxxo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7478455047338214418', 'uniqueId': 'xddelosxd', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/c20bfec948f7f0b66cab624ba8ed05e8~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=6f5855fc&amp;x-expires=1760619600&amp;x-signature=gLZIHwQiqJjv2RD%2BUKE%2FTcNaTgw%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3056,25 +3056,25 @@
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>ya los tengo</t>
+          <t>18,4</t>
         </is>
       </c>
       <c r="G47" s="2" t="n">
-        <v>45930.06351851852</v>
+        <v>45942.79722222222</v>
       </c>
       <c r="H47" s="3" t="n">
-        <v>45930</v>
+        <v>45942</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>01:31:28</t>
+          <t>19:08:00</t>
         </is>
       </c>
       <c r="J47" t="n">
         <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" t="b">
         <v>0</v>
@@ -3086,7 +3086,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555688754276303624', 'createTime': 1759195888, 'createTimeISO': '2025-09-30T01:31:28.000Z', 'text': 'ya los tengo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7506596631263200262', 'uniqueId': 'mi.princesa.divin', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/c158a0051a2d172e45e96e5273f348d8~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=16b91f19&amp;x-expires=1759593600&amp;x-signature=%2FBRermlmFUha%2BdfPHbvfTM07W%2FE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7560414054448366354', 'createTime': 1760296080, 'createTimeISO': '2025-10-12T19:08:00.000Z', 'text': '18,4', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7381118081303659525', 'uniqueId': 'jose.augusto.palo3', 'avatarThumbnail': 'https://p77-sign-va.tiktokcdn.com/tos-maliva-avt-0068/69ab084a6c804d04957ca1b46da752e7~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=c4deac63&amp;x-expires=1760619600&amp;x-signature=tBjBOiPBcsdiaUQLgI0V1R3xtwQ%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3112,18 +3112,18 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>yo tengo el azul 🥹🥹🥹</t>
+          <t>En cucuta no hay</t>
         </is>
       </c>
       <c r="G48" s="2" t="n">
-        <v>45927.73127314815</v>
+        <v>45938.6677662037</v>
       </c>
       <c r="H48" s="3" t="n">
-        <v>45927</v>
+        <v>45938</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>17:33:02</t>
+          <t>16:01:35</t>
         </is>
       </c>
       <c r="J48" t="n">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554823300175905544', 'createTime': 1758994382, 'createTimeISO': '2025-09-27T17:33:02.000Z', 'text': 'yo tengo el azul \U0001f979\U0001f979\U0001f979', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7357836616147059717', 'uniqueId': 'kako.hemilio', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/1760399f4c117a473725b3bb20f7bf21~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=3148a253&amp;x-expires=1759593600&amp;x-signature=newLH70ZekNand6GTZVaSP338hc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7558881690249396999', 'createTime': 1759939295, 'createTimeISO': '2025-10-08T16:01:35.000Z', 'text': 'En cucuta no hay', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7209509026618950662', 'uniqueId': 'user924075672', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/dc5cae3865198f457d7af8926610de21~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=2ff94603&amp;x-expires=1760619600&amp;x-signature=B%2BkGgPblEe44%2BSKF%2Bt4wZEef5oQ%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=my2', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3168,25 +3168,25 @@
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
-          <t>a qui no hay</t>
+          <t>saquen ya otra colección 😕</t>
         </is>
       </c>
       <c r="G49" s="2" t="n">
-        <v>45929.99042824074</v>
+        <v>45926.96346064815</v>
       </c>
       <c r="H49" s="3" t="n">
-        <v>45929</v>
+        <v>45926</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>23:46:13</t>
+          <t>23:07:23</t>
         </is>
       </c>
       <c r="J49" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K49" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L49" t="b">
         <v>0</v>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555661409931330305', 'createTime': 1759189573, 'createTimeISO': '2025-09-29T23:46:13.000Z', 'text': 'a qui no hay', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7142647410137138181', 'uniqueId': 'arsel9324', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/5120f48c75061dc7b3c9c01722658d71~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=46eb09da&amp;x-expires=1759593600&amp;x-signature=RPVu0oXRnEm1Gxrj9OUcBof4hKw%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554538366990189319', 'createTime': 1758928043, 'createTimeISO': '2025-09-26T23:07:23.000Z', 'text': 'saquen ya otra colección 😕', 'diggCount': 3, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 6, 'uid': '7430556660474758150', 'uniqueId': 'esobrad_1', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/496be0dadae6d46720222260f6036998~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=4de75e78&amp;x-expires=1760619600&amp;x-signature=m%2Ffa9GB1DhFhrAOslsYL0%2BBUM4U%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3224,22 +3224,22 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>yo los tengo tengo el rosado y el azul</t>
+          <t>y si tengo repetidos no me los cambian 😂😂</t>
         </is>
       </c>
       <c r="G50" s="2" t="n">
-        <v>45928.95548611111</v>
+        <v>45926.88744212963</v>
       </c>
       <c r="H50" s="3" t="n">
-        <v>45928</v>
+        <v>45926</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>22:55:54</t>
+          <t>21:17:55</t>
         </is>
       </c>
       <c r="J50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" t="n">
         <v>0</v>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555277557701575431', 'createTime': 1759100154, 'createTimeISO': '2025-09-28T22:55:54.000Z', 'text': 'yo los tengo tengo el rosado y el azul', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7541992424257324053', 'uniqueId': 'lamasquedoradora', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/29368d9813b06794e313abee8fbbb2d1~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=0b3d479b&amp;x-expires=1759593600&amp;x-signature=A5p%2BBJ29DX2PLJEP9yWspQio4sM%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554510104642650896', 'createTime': 1758921475, 'createTimeISO': '2025-09-26T21:17:55.000Z', 'text': 'y si tengo repetidos no me los cambian 😂😂', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6835450069409514502', 'uniqueId': 'ailatanollirum', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/474f3a22808ad684a516e4b07cab2a37~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=5bd3d40b&amp;x-expires=1760619600&amp;x-signature=gFmEFs4NEyN8TRgN7fRFkyCTtHs%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3280,22 +3280,22 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>yo ya tengo esa m</t>
+          <t>tengo un montón de Mochis de la primera colección, valdrá mucho?</t>
         </is>
       </c>
       <c r="G51" s="2" t="n">
-        <v>45929.65525462963</v>
+        <v>45926.67013888889</v>
       </c>
       <c r="H51" s="3" t="n">
-        <v>45929</v>
+        <v>45926</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>15:43:34</t>
+          <t>16:05:00</t>
         </is>
       </c>
       <c r="J51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" t="n">
         <v>0</v>
@@ -3310,7 +3310,7 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555537273380815623', 'createTime': 1759160614, 'createTimeISO': '2025-09-29T15:43:34.000Z', 'text': 'yo ya tengo esa m', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7470382147061777409', 'uniqueId': 'thaly1772', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/71e85da6987e62511391075c6d6674c0~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=e122dbe5&amp;x-expires=1759593600&amp;x-signature=gxLDjAHbEGYidQPyFuvswX3BReU%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554429537663386376', 'createTime': 1758902700, 'createTimeISO': '2025-09-26T16:05:00.000Z', 'text': 'tengo un montón de Mochis de la primera colección, valdrá mucho?', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7116292147141166086', 'uniqueId': 'just_fenix67', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/9270efdc513746d459737e05d9dccbee~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=3ad418fa&amp;x-expires=1760619600&amp;x-signature=I3FASPimihdwxr84fHBdxfdmMzs%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3336,25 +3336,25 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>En Neiva no hay oxxo 😭</t>
+          <t>y si ya corte los logos y no dice mochi saurios y ya vote el empaque con el qr</t>
         </is>
       </c>
       <c r="G52" s="2" t="n">
-        <v>45927.72614583333</v>
+        <v>45927.05542824074</v>
       </c>
       <c r="H52" s="3" t="n">
         <v>45927</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>17:25:39</t>
+          <t>01:19:49</t>
         </is>
       </c>
       <c r="J52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L52" t="b">
         <v>0</v>
@@ -3366,7 +3366,7 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554821395772867335', 'createTime': 1758993939, 'createTimeISO': '2025-09-27T17:25:39.000Z', 'text': 'En Neiva no hay oxxo 😭', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7119701816863065094', 'uniqueId': 'lucy_kitty115', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/28e44ab8ed2a9fc54365bb88cdd438e4~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=8cdfa3b5&amp;x-expires=1759593600&amp;x-signature=mRIERMgLS3IBX40VsJ6V4rwofBo%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554572506653803272', 'createTime': 1758935989, 'createTimeISO': '2025-09-27T01:19:49.000Z', 'text': 'y si ya corte los logos y no dice mochi saurios y ya vote el empaque con el qr', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6887020420505109509', 'uniqueId': 'mari_a0131', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/52b610568365088bb8157c0e968fb5e0~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=e0711180&amp;x-expires=1760619600&amp;x-signature=NeeBDtvo2RrlmPS7IYZg6k42kgc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3392,25 +3392,26 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>en santander no hay oxxo😭😭😭😭😭😭</t>
+          <t>Por que en oxxo por que e
+En Colombia no hay tantos oxxos</t>
         </is>
       </c>
       <c r="G53" s="2" t="n">
-        <v>45927.72530092593</v>
+        <v>45930.00252314815</v>
       </c>
       <c r="H53" s="3" t="n">
-        <v>45927</v>
+        <v>45930</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>17:24:26</t>
+          <t>00:03:38</t>
         </is>
       </c>
       <c r="J53" t="n">
         <v>0</v>
       </c>
       <c r="K53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53" t="b">
         <v>0</v>
@@ -3422,7 +3423,7 @@
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554821062325453584', 'createTime': 1758993866, 'createTimeISO': '2025-09-27T17:24:26.000Z', 'text': 'en santander no hay oxxo😭😭😭😭😭😭', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7378516455367279622', 'uniqueId': 'pablo.andres.grij', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/be54fa419e20e6530484a6289699c5e3~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=b5dbe348&amp;x-expires=1759593600&amp;x-signature=g0reZhJGwlWUUmc7H3tPYIjf5a0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555666073921553160', 'createTime': 1759190618, 'createTimeISO': '2025-09-30T00:03:38.000Z', 'text': 'Por que en oxxo por que e\nEn Colombia no hay tantos oxxos', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7433071984395338758', 'uniqueId': 'viky1234836', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/f814e9b802ec7cd1d5d09a202afca7a9~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=3e1568c8&amp;x-expires=1760619600&amp;x-signature=NZ8T6fe9stxxeX2UGhgEcqrHH6g%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3448,25 +3449,25 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>en pasto no ay oxxo</t>
+          <t>en muchos lugares no hay Oxxo no pensaron en nosotros</t>
         </is>
       </c>
       <c r="G54" s="2" t="n">
-        <v>45927.67798611111</v>
+        <v>45929.99023148148</v>
       </c>
       <c r="H54" s="3" t="n">
-        <v>45927</v>
+        <v>45929</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>16:16:18</t>
+          <t>23:45:56</t>
         </is>
       </c>
       <c r="J54" t="n">
         <v>0</v>
       </c>
       <c r="K54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L54" t="b">
         <v>0</v>
@@ -3478,7 +3479,7 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554803546690077447', 'createTime': 1758989778, 'createTimeISO': '2025-09-27T16:16:18.000Z', 'text': 'en pasto no ay oxxo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7478455047338214418', 'uniqueId': 'xddelosxd', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/522f653962a9c5f393bbac9e902ed8d8~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=1798c426&amp;x-expires=1759593600&amp;x-signature=8tmHisc5uSF2QdqnUVxmc8mo6XA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555661460748206849', 'createTime': 1759189556, 'createTimeISO': '2025-09-29T23:45:56.000Z', 'text': 'en muchos lugares no hay Oxxo no pensaron en nosotros', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7142647410137138181', 'uniqueId': 'arsel9324', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/50fc02d856bc86dadfa85351b5eebcde~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=3ec46f77&amp;x-expires=1760619600&amp;x-signature=bc2ui9k%2FpKLOUdvXx39v7r15AhY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3504,25 +3505,25 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Los quieroooooo</t>
+          <t>en colombia noa ah</t>
         </is>
       </c>
       <c r="G55" s="2" t="n">
-        <v>45929.49574074074</v>
+        <v>45926.84263888889</v>
       </c>
       <c r="H55" s="3" t="n">
-        <v>45929</v>
+        <v>45926</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>11:53:52</t>
+          <t>20:13:24</t>
         </is>
       </c>
       <c r="J55" t="n">
         <v>0</v>
       </c>
       <c r="K55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55" t="b">
         <v>0</v>
@@ -3534,7 +3535,7 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555478087270515477', 'createTime': 1759146832, 'createTimeISO': '2025-09-29T11:53:52.000Z', 'text': 'Los quieroooooo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '6886209614263403522', 'uniqueId': 'mariajose.jr0214', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/fa89b236738521d8d51d425df266db3b~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=1c0da65c&amp;x-expires=1759593600&amp;x-signature=78h1OzcVZD8rneI%2F8ybr1mWRgxs%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554493529289638664', 'createTime': 1758917604, 'createTimeISO': '2025-09-26T20:13:24.000Z', 'text': 'en colombia noa ah', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7503310884556309511', 'uniqueId': 'alba_hernandez21', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/3081f3280dc30ced6c73649afc9e82b1~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=b8419c34&amp;x-expires=1760619600&amp;x-signature=%2B4CF6ZJwvXwPBXhPx0XoSHlKpMc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3560,18 +3561,18 @@
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Va uno al Oxxo y qué no han llegado. No todas las tiendas tienen ese empaque marcado, tanto misterio para un muñeco, antes eran 3 logos ahora 4. Mejor me compro una Drácula</t>
+          <t>part 2</t>
         </is>
       </c>
       <c r="G56" s="2" t="n">
-        <v>45933.15829861111</v>
+        <v>45929.57021990741</v>
       </c>
       <c r="H56" s="3" t="n">
-        <v>45933</v>
+        <v>45929</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>03:47:57</t>
+          <t>13:41:07</t>
         </is>
       </c>
       <c r="J56" t="n">
@@ -3590,7 +3591,7 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556837188043227905', 'createTime': 1759463277, 'createTimeISO': '2025-10-03T03:47:57.000Z', 'text': 'Va uno al Oxxo y qué no han llegado. No todas las tiendas tienen ese empaque marcado, tanto misterio para un muñeco, antes eran 3 logos ahora 4. Mejor me compro una Drácula', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6798221952290964486', 'uniqueId': 'pizpir_', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/7331755100833644549~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=6c9a8094&amp;x-expires=1759593600&amp;x-signature=MgvSjjxdng3lAL5qMpVcCa0MGE0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555505705790538514', 'createTime': 1759153267, 'createTimeISO': '2025-09-29T13:41:07.000Z', 'text': 'part 2', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7518189866266526728', 'uniqueId': 'jenny.loango', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/0aa7aaecbe34f7dd94d1887fac659dec~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=774ddd4b&amp;x-expires=1760619600&amp;x-signature=yLnrAheaWHXl%2FP2t6K5mkKCJgBg%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3616,18 +3617,18 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>yo tengo el moradoro y el verde y otro morado que es igual al verde Pero morado y voy a ir al Oxxo que queda cerca de mi casa y reclamo varios ksjsjsjs</t>
+          <t>Ay yo pensaba que ya se avía acabado y tambien pensaba que ya no tenía oportunidad de reclamar mis 12 tarjetas y como 7 logos 😭😭😭😔</t>
         </is>
       </c>
       <c r="G57" s="2" t="n">
-        <v>45933.44353009259</v>
+        <v>45935.67759259259</v>
       </c>
       <c r="H57" s="3" t="n">
-        <v>45933</v>
+        <v>45935</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>10:38:41</t>
+          <t>16:15:44</t>
         </is>
       </c>
       <c r="J57" t="n">
@@ -3646,7 +3647,7 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556943055979332372', 'createTime': 1759487921, 'createTimeISO': '2025-10-03T10:38:41.000Z', 'text': 'yo tengo el moradoro y el verde y otro morado que es igual al verde Pero morado y voy a ir al Oxxo que queda cerca de mi casa y reclamo varios ksjsjsjs', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7529200266735715346', 'uniqueId': 'gabriela__gomez_valencia', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/e22b97238fcbe193cfd4126cef752c6d~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=483edc42&amp;x-expires=1759593600&amp;x-signature=2dCsXdsu%2BwI8hKgp8x0keOfjkl4%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7557772077760742152', 'createTime': 1759680944, 'createTimeISO': '2025-10-05T16:15:44.000Z', 'text': 'Ay yo pensaba que ya se avía acabado y tambien pensaba que ya no tenía oportunidad de reclamar mis 12 tarjetas y como 7 logos 😭😭😭😔', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7538082276980737029', 'uniqueId': 'mariiladiva0', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/8ede218c4c09353a38122ea601611b79~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=31cb7408&amp;x-expires=1760619600&amp;x-signature=1hsNYLQnM0OD%2BXKjhibdnpYx1l0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3672,18 +3673,18 @@
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>y para que sirve eso, que beneficios tiene 😳</t>
+          <t>Yo ya los tengo los logos</t>
         </is>
       </c>
       <c r="G58" s="2" t="n">
-        <v>45933.05707175926</v>
+        <v>45934.66412037037</v>
       </c>
       <c r="H58" s="3" t="n">
-        <v>45933</v>
+        <v>45934</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>01:22:11</t>
+          <t>15:56:20</t>
         </is>
       </c>
       <c r="J58" t="n">
@@ -3702,7 +3703,7 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556799608577458951', 'createTime': 1759454531, 'createTimeISO': '2025-10-03T01:22:11.000Z', 'text': 'y para que sirve eso, que beneficios tiene 😳', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6935601595720860678', 'uniqueId': 'monica_lenis1980', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/fce7942c402b7371d210f51cf61e58d9~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=b8b54604&amp;x-expires=1759593600&amp;x-signature=rbDOJQKkh4KdQyG7YEaDALYqAW8%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7557395985225335570', 'createTime': 1759593380, 'createTimeISO': '2025-10-04T15:56:20.000Z', 'text': 'Yo ya los tengo los logos', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7364207363702047750', 'uniqueId': 'lady.insuasti', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/567cb1b8e1d71f6af4d01946884814a5~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=6aed58c4&amp;x-expires=1760619600&amp;x-signature=lqXKFpKo3OkC4RkMsUrlhySr6jE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3728,22 +3729,22 @@
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>oigan pero no encuentro mochisaurios solo ilumimochis</t>
+          <t>yo lo consigo en una papelera sin comprar el yogur</t>
         </is>
       </c>
       <c r="G59" s="2" t="n">
-        <v>45932.81353009259</v>
+        <v>45930.02420138889</v>
       </c>
       <c r="H59" s="3" t="n">
-        <v>45932</v>
+        <v>45930</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>19:31:29</t>
+          <t>00:34:51</t>
         </is>
       </c>
       <c r="J59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K59" t="n">
         <v>0</v>
@@ -3758,7 +3759,7 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556709242481722130', 'createTime': 1759433489, 'createTimeISO': '2025-10-02T19:31:29.000Z', 'text': 'oigan pero no encuentro mochisaurios solo ilumimochis', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7121425545787868165', 'uniqueId': 'filosofia.gatuna', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/611472f8abb9c3c4e66c407a80c4ee1b~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=83c0e8e3&amp;x-expires=1759593600&amp;x-signature=mWo16yzRG4TOkkujvdiwZi2tY%2Bo%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555674134270001927', 'createTime': 1759192491, 'createTimeISO': '2025-09-30T00:34:51.000Z', 'text': 'yo lo consigo en una papelera sin comprar el yogur', 'diggCount': 1, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7384092541786014725', 'uniqueId': 'estrellita_alien', 'avatarThumbnail': 'https://p19-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/e38c298456b8a03417d891b1539c5b57~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=4752d593&amp;x-expires=1760619600&amp;x-signature=v5chIa6fC%2F8UKQt%2Fnu4OQh67QJY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3784,18 +3785,18 @@
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>mano me compré uno y me salió un unicornio</t>
+          <t>Va uno al Oxxo y qué no han llegado. No todas las tiendas tienen ese empaque marcado, tanto misterio para un muñeco, antes eran 3 logos ahora 4. Mejor me compro una Drácula</t>
         </is>
       </c>
       <c r="G60" s="2" t="n">
-        <v>45933.02133101852</v>
+        <v>45933.15829861111</v>
       </c>
       <c r="H60" s="3" t="n">
         <v>45933</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>00:30:43</t>
+          <t>03:47:57</t>
         </is>
       </c>
       <c r="J60" t="n">
@@ -3814,7 +3815,7 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556786291250725633', 'createTime': 1759451443, 'createTimeISO': '2025-10-03T00:30:43.000Z', 'text': 'mano me compré uno y me salió un unicornio', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7076201709093749765', 'uniqueId': 'bloom_xs01', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/7841c743cce7ed0aeb6a326261626994~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=0f5e04c5&amp;x-expires=1759593600&amp;x-signature=8jIw9LLwJrwn5zlZRntxz3SrO8A%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556837188043227905', 'createTime': 1759463277, 'createTimeISO': '2025-10-03T03:47:57.000Z', 'text': 'Va uno al Oxxo y qué no han llegado. No todas las tiendas tienen ese empaque marcado, tanto misterio para un muñeco, antes eran 3 logos ahora 4. Mejor me compro una Drácula', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6798221952290964486', 'uniqueId': 'pizpir_', 'avatarThumbnail': 'https://p19-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/7331755100833644549~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=d4d1f41f&amp;x-expires=1760619600&amp;x-signature=E5kP34mziAd0zcs7mO5Rcx%2B4rfQ%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3840,18 +3841,18 @@
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>ayer compré el yogo premio con la etiqueta de mochisaurios mi hijo con ilusión lo abrió y va y le sale de la coleccion pasada....Nooo así si nooo al menos quiten los de la coleccion pasada para que no pase esto</t>
         </is>
       </c>
       <c r="G61" s="2" t="n">
-        <v>45928.80891203704</v>
+        <v>45929.88107638889</v>
       </c>
       <c r="H61" s="3" t="n">
-        <v>45928</v>
+        <v>45929</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>19:24:50</t>
+          <t>21:08:45</t>
         </is>
       </c>
       <c r="J61" t="n">
@@ -3870,7 +3871,7 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555223199790154503', 'createTime': 1759087490, 'createTimeISO': '2025-09-28T19:24:50.000Z', 'text': 'ok', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6987105799349847046', 'uniqueId': 'dahyun_mi_esposa033', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/b2f50854382d6b9422d13f90900f75a2~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=78a579ca&amp;x-expires=1759593600&amp;x-signature=GjYy1ASDIYAH7PfB6nSC9qeZaLw%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555620990967153409', 'createTime': 1759180125, 'createTimeISO': '2025-09-29T21:08:45.000Z', 'text': 'ayer compré el yogo premio con la etiqueta de mochisaurios mi hijo con ilusión lo abrió y va y le sale de la coleccion pasada....Nooo así si nooo al menos quiten los de la coleccion pasada para que no pase esto', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6846492796284470277', 'uniqueId': 'linamariahernan4', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/b8c84acbfe31152b7111b26ebbb541b5~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=b9f8bdf6&amp;x-expires=1760619600&amp;x-signature=pfQeFe3JOjhTpmxwnJxKnu3EHsI%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3896,18 +3897,18 @@
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Tanta cosa para uno</t>
+          <t>eran mejor los gogos</t>
         </is>
       </c>
       <c r="G62" s="2" t="n">
-        <v>45929.00190972222</v>
+        <v>45929.47387731481</v>
       </c>
       <c r="H62" s="3" t="n">
         <v>45929</v>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>00:02:45</t>
+          <t>11:22:23</t>
         </is>
       </c>
       <c r="J62" t="n">
@@ -3926,7 +3927,7 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555294742864954119', 'createTime': 1759104165, 'createTimeISO': '2025-09-29T00:02:45.000Z', 'text': 'Tanta cosa para uno', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7243912158169465862', 'uniqueId': 'aguiilarpaolita', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/28050a045b8ba65347a8d82eb886b7be~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=4346e872&amp;x-expires=1759593600&amp;x-signature=5DkD2YxvDbU5odzhlVCeIkiJd7k%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555469953446052609', 'createTime': 1759144943, 'createTimeISO': '2025-09-29T11:22:23.000Z', 'text': 'eran mejor los gogos', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7228579787227350022', 'uniqueId': 'diazsergio448', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/61df6591ddc0252c4f89c7801a873c3c~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=ef7233fd&amp;x-expires=1760619600&amp;x-signature=IM6jnH7FW%2FlK0X4Vstlk%2B9IK9Vg%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -3952,18 +3953,18 @@
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
-          <t>y las ciudades donde no hay Oxxo 😅😅</t>
+          <t>QUE CALIDAD🗣️🗣️🗣</t>
         </is>
       </c>
       <c r="G63" s="2" t="n">
-        <v>45927.13207175926</v>
+        <v>45929.74858796296</v>
       </c>
       <c r="H63" s="3" t="n">
-        <v>45927</v>
+        <v>45929</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>03:10:11</t>
+          <t>17:57:58</t>
         </is>
       </c>
       <c r="J63" t="n">
@@ -3982,7 +3983,7 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554600954244678407', 'createTime': 1758942611, 'createTimeISO': '2025-09-27T03:10:11.000Z', 'text': 'y las ciudades donde no hay Oxxo 😅😅', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6783394257204282373', 'uniqueId': 'yunior.18', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/b9b4e3df13da81e5d8bd40873e3374d1~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=4ec8d068&amp;x-expires=1759593600&amp;x-signature=0fnUVWhf0wNsaEKewxF2eM8s3gE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555571878653592340', 'createTime': 1759168678, 'createTimeISO': '2025-09-29T17:57:58.000Z', 'text': 'QUE CALIDAD🗣️🗣️🗣', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7458314603111613446', 'uniqueId': 'como.quieran.quie', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/9fb7f4d59fb4cd488465c38f8b999208~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=a41528b4&amp;x-expires=1760619600&amp;x-signature=QN3a%2F%2BaN%2BkC%2BvaZxPlqx0uxk634%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4008,18 +4009,18 @@
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
-          <t>me puede regalar la cámara</t>
+          <t>eso pa que</t>
         </is>
       </c>
       <c r="G64" s="2" t="n">
-        <v>45927.25508101852</v>
+        <v>45928.22596064815</v>
       </c>
       <c r="H64" s="3" t="n">
-        <v>45927</v>
+        <v>45928</v>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>06:07:19</t>
+          <t>05:25:23</t>
         </is>
       </c>
       <c r="J64" t="n">
@@ -4038,7 +4039,7 @@
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554646606097629960', 'createTime': 1758953239, 'createTimeISO': '2025-09-27T06:07:19.000Z', 'text': 'me puede regalar la cámara', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7359244510582670341', 'uniqueId': 'fernando.bertho', 'avatarThumbnail': 'https://p19-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/7359244971364319238~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=9bdd8bdf&amp;x-expires=1759593600&amp;x-signature=UaThl4fOZHF%2Fb5HdkgdJi4ZT7nk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555006889290826503', 'createTime': 1759037123, 'createTimeISO': '2025-09-28T05:25:23.000Z', 'text': 'eso pa que', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7542870679370417160', 'uniqueId': 'x_xxx660', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/baad79b549774584b1a67ebfc08f5a67~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=e29e0891&amp;x-expires=1760619600&amp;x-signature=6sXvI1XTtEDbwtXpLSnjXPSWsbQ%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4064,18 +4065,18 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Los Amooo pero Uyy un montón de cosas para el recambio!</t>
+          <t>yo los tengo tengo el rosado y el azul</t>
         </is>
       </c>
       <c r="G65" s="2" t="n">
-        <v>45927.14011574074</v>
+        <v>45928.95548611111</v>
       </c>
       <c r="H65" s="3" t="n">
-        <v>45927</v>
+        <v>45928</v>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>03:21:46</t>
+          <t>22:55:54</t>
         </is>
       </c>
       <c r="J65" t="n">
@@ -4094,7 +4095,7 @@
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554603916571640577', 'createTime': 1758943306, 'createTimeISO': '2025-09-27T03:21:46.000Z', 'text': 'Los Amooo pero Uyy un montón de cosas para el recambio!', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7496003126047851521', 'uniqueId': 'caroprietog', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/2a832b79f12188da997912c7d49288a5~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=0a7d49dc&amp;x-expires=1759593600&amp;x-signature=7swUn2mleuHXHUgbLUz6rSgpRVM%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555277557701575431', 'createTime': 1759100154, 'createTimeISO': '2025-09-28T22:55:54.000Z', 'text': 'yo los tengo tengo el rosado y el azul', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7541992424257324053', 'uniqueId': 'lamasquedoradora', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/29368d9813b06794e313abee8fbbb2d1~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=41244ad2&amp;x-expires=1760619600&amp;x-signature=gZ%2Fik1ZEQc%2Bq6ciT67m2IYVQ76w%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4120,18 +4121,18 @@
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
-          <t>ayer compré el yogo premio con la etiqueta de mochisaurios mi hijo con ilusión lo abrió y va y le sale de la coleccion pasada....Nooo así si nooo al menos quiten los de la coleccion pasada para que no pase esto</t>
+          <t>si claro si yo vivo en colomb</t>
         </is>
       </c>
       <c r="G66" s="2" t="n">
-        <v>45929.88107638889</v>
+        <v>45930.02231481481</v>
       </c>
       <c r="H66" s="3" t="n">
-        <v>45929</v>
+        <v>45930</v>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>21:08:45</t>
+          <t>00:32:08</t>
         </is>
       </c>
       <c r="J66" t="n">
@@ -4150,7 +4151,7 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555620990967153409', 'createTime': 1759180125, 'createTimeISO': '2025-09-29T21:08:45.000Z', 'text': 'ayer compré el yogo premio con la etiqueta de mochisaurios mi hijo con ilusión lo abrió y va y le sale de la coleccion pasada....Nooo así si nooo al menos quiten los de la coleccion pasada para que no pase esto', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6846492796284470277', 'uniqueId': 'linamariahernan4', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/b8c84acbfe31152b7111b26ebbb541b5~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=512bf77d&amp;x-expires=1759593600&amp;x-signature=xX7e33oEx1QtyVAuRhbxGCANd20%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555673462803694343', 'createTime': 1759192328, 'createTimeISO': '2025-09-30T00:32:08.000Z', 'text': 'si claro si yo vivo en colomb', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7552728943149810705', 'uniqueId': 'dannasofi6899', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/865736a245746c0e4f5e41bb7590a553~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=fcb4408f&amp;x-expires=1760619600&amp;x-signature=AsnCa1SW58CsnRbl1FwmMbxkYB8%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4206,7 +4207,7 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554575152081535765', 'createTime': 1758936609, 'createTimeISO': '2025-09-27T01:30:09.000Z', 'text': 'ami me salió un cocodrilo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6882570284298142721', 'uniqueId': 'cubides08', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/55f4e79659fb01bed4bf116832dd843d~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=9c38d185&amp;x-expires=1759593600&amp;x-signature=o1kMZPa3Z0an7GNWv%2BLc53XFlqo%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554575152081535765', 'createTime': 1758936609, 'createTimeISO': '2025-09-27T01:30:09.000Z', 'text': 'ami me salió un cocodrilo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6882570284298142721', 'uniqueId': 'cubides08', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/55f4e79659fb01bed4bf116832dd843d~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=d289249c&amp;x-expires=1760619600&amp;x-signature=H1CdHqE1dOUp7oMPrA6hTYJiGNg%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4232,18 +4233,18 @@
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
-          <t>y las lavadoras?</t>
+          <t>una pregunta soy de Colombia pero vivo en un lugar un poco lejos 🥺 cuando llegan es Arauca</t>
         </is>
       </c>
       <c r="G68" s="2" t="n">
-        <v>45926.92902777778</v>
+        <v>45928.79006944445</v>
       </c>
       <c r="H68" s="3" t="n">
-        <v>45926</v>
+        <v>45928</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>22:17:48</t>
+          <t>18:57:42</t>
         </is>
       </c>
       <c r="J68" t="n">
@@ -4262,7 +4263,7 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554525489421386516', 'createTime': 1758925068, 'createTimeISO': '2025-09-26T22:17:48.000Z', 'text': 'y las lavadoras?', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7390524142800667653', 'uniqueId': 'trululxx', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/efcb9ba983ceef1f1798cb089ff26aa8~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=0109ecd5&amp;x-expires=1759593600&amp;x-signature=mcius3P7IGwAUScDihCz8rnlnMQ%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555216216953078536', 'createTime': 1759085862, 'createTimeISO': '2025-09-28T18:57:42.000Z', 'text': 'una pregunta soy de Colombia pero vivo en un lugar un poco lejos 🥺 cuando llegan es Arauca', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7514280435070927873', 'uniqueId': 'fresa.com.crema', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/eaa3b275b74194b2e13fc3266612bc49~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=f3263ab8&amp;x-expires=1760619600&amp;x-signature=KnPU9CErD%2FcTZYaJ6ZdbJOwcZ8A%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4288,18 +4289,18 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>son mejores los de colanta</t>
+          <t>do</t>
         </is>
       </c>
       <c r="G69" s="2" t="n">
-        <v>45928.76954861111</v>
+        <v>45936.66792824074</v>
       </c>
       <c r="H69" s="3" t="n">
-        <v>45928</v>
+        <v>45936</v>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>18:28:09</t>
+          <t>16:01:49</t>
         </is>
       </c>
       <c r="J69" t="n">
@@ -4318,7 +4319,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555208572725822228', 'createTime': 1759084089, 'createTimeISO': '2025-09-28T18:28:09.000Z', 'text': 'son mejores los de colanta', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6970094734828438533', 'uniqueId': 'videosdehumornegro', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/3d43f03cc0c977cda48bd3640cc5246a~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=2a88e569&amp;x-expires=1759593600&amp;x-signature=2CeDShrAgfmB3jryls18vK8U3Xs%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7558139554667299585', 'createTime': 1759766509, 'createTimeISO': '2025-10-06T16:01:49.000Z', 'text': 'do', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7347759303850460166', 'uniqueId': 'daniel.medina9402', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/d827ef96dbb9538e76ca4c0a1031de75~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=6d689b7d&amp;x-expires=1760619600&amp;x-signature=wUzyOig0YQcBHe1a%2FA5mb3ZJpRM%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4344,18 +4345,18 @@
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
-          <t>una pregunta soy de Colombia pero vivo en un lugar un poco lejos 🥺 cuando llegan es Arauca</t>
+          <t>Amooo</t>
         </is>
       </c>
       <c r="G70" s="2" t="n">
-        <v>45928.79006944445</v>
+        <v>45928.79438657407</v>
       </c>
       <c r="H70" s="3" t="n">
         <v>45928</v>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>18:57:42</t>
+          <t>19:03:55</t>
         </is>
       </c>
       <c r="J70" t="n">
@@ -4374,7 +4375,7 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555216216953078536', 'createTime': 1759085862, 'createTimeISO': '2025-09-28T18:57:42.000Z', 'text': 'una pregunta soy de Colombia pero vivo en un lugar un poco lejos 🥺 cuando llegan es Arauca', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7514280435070927873', 'uniqueId': 'fresa.com.crema', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/eaa3b275b74194b2e13fc3266612bc49~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=ad885e61&amp;x-expires=1759593600&amp;x-signature=tc0mwzUbT9JqWSR5%2FCwhl%2FFnYr0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555217811128615687', 'createTime': 1759086235, 'createTimeISO': '2025-09-28T19:03:55.000Z', 'text': 'Amooo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7284419691349607430', 'uniqueId': 'kdruiz22', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/7300345897722839046~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=e66026c4&amp;x-expires=1760619600&amp;x-signature=lPpueY4D39QKi7BZTOG96veKUac%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4400,19 +4401,18 @@
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Por que en oxxo por que e
-En Colombia no hay tantos oxxos</t>
+          <t>mi mala suerte, tenía dos abri un yogurt y me salió repetido</t>
         </is>
       </c>
       <c r="G71" s="2" t="n">
-        <v>45930.00252314815</v>
+        <v>45928.00234953704</v>
       </c>
       <c r="H71" s="3" t="n">
-        <v>45930</v>
+        <v>45928</v>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>00:03:38</t>
+          <t>00:03:23</t>
         </is>
       </c>
       <c r="J71" t="n">
@@ -4431,7 +4431,7 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555666073921553160', 'createTime': 1759190618, 'createTimeISO': '2025-09-30T00:03:38.000Z', 'text': 'Por que en oxxo por que e\nEn Colombia no hay tantos oxxos', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7433071984395338758', 'uniqueId': 'viky1234836', 'avatarThumbnail': 'https://p19-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/d5790da85f33c83b665c0f5cdae82ee1~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=7eb79533&amp;x-expires=1759593600&amp;x-signature=YU8IEn82b605XKLDcxzzDUexwes%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554923850959422215', 'createTime': 1759017803, 'createTimeISO': '2025-09-28T00:03:23.000Z', 'text': 'mi mala suerte, tenía dos abri un yogurt y me salió repetido', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7540478701881164818', 'uniqueId': 'cib_1252', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/c44cc5b4ca1d9f823d88604b1f5d3cfd~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=21c58c91&amp;x-expires=1760619600&amp;x-signature=uPXR7yaqtQa%2BwIViex8Hz1dxel4%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4457,18 +4457,18 @@
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
-          <t>ya se dieron cuenta que Coca-Cola trajo nuevamente los hielocos.</t>
+          <t>no los venden? saldría más económico.</t>
         </is>
       </c>
       <c r="G72" s="2" t="n">
-        <v>45928.82883101852</v>
+        <v>45942.93608796296</v>
       </c>
       <c r="H72" s="3" t="n">
-        <v>45928</v>
+        <v>45942</v>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>19:53:31</t>
+          <t>22:27:58</t>
         </is>
       </c>
       <c r="J72" t="n">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555230564963648264', 'createTime': 1759089211, 'createTimeISO': '2025-09-28T19:53:31.000Z', 'text': 'ya se dieron cuenta que Coca-Cola trajo nuevamente los hielocos.', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7311721551714796549', 'uniqueId': 'junior.xd.velez', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/7311721679486386181~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=b437b32a&amp;x-expires=1759593600&amp;x-signature=js0MP0HUQZ8rh%2BFKcmvsRQiHU2o%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7560465563730920199', 'createTime': 1760308078, 'createTimeISO': '2025-10-12T22:27:58.000Z', 'text': 'no los venden? saldría más económico.', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6900093665232208898', 'uniqueId': 'alonsocastaeda4', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/656e080d9831aeebef39b67358dbf496~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=a766fb9a&amp;x-expires=1760619600&amp;x-signature=8G%2FEU3VEKd1u9Sy8r6E9NBUdU6g%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4513,25 +4513,25 @@
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>en muchos lugares no hay Oxxo no pensaron en nosotros</t>
+          <t>y si estoy en Colombia</t>
         </is>
       </c>
       <c r="G73" s="2" t="n">
-        <v>45929.99023148148</v>
+        <v>45930.03666666667</v>
       </c>
       <c r="H73" s="3" t="n">
-        <v>45929</v>
+        <v>45930</v>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>23:45:56</t>
+          <t>00:52:48</t>
         </is>
       </c>
       <c r="J73" t="n">
         <v>0</v>
       </c>
       <c r="K73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L73" t="b">
         <v>0</v>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555661460748206849', 'createTime': 1759189556, 'createTimeISO': '2025-09-29T23:45:56.000Z', 'text': 'en muchos lugares no hay Oxxo no pensaron en nosotros', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7142647410137138181', 'uniqueId': 'arsel9324', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/5120f48c75061dc7b3c9c01722658d71~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=753b8b84&amp;x-expires=1759593600&amp;x-signature=%2BwOL3I77ZpqVBCcLvsgra6O8U3E%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555678757781422856', 'createTime': 1759193568, 'createTimeISO': '2025-09-30T00:52:48.000Z', 'text': 'y si estoy en Colombia', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7511370345698526228', 'uniqueId': 'eslendy121', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/12ff77457a3980c682406f9a561bcfdc~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=d48f7f70&amp;x-expires=1760619600&amp;x-signature=VDEwGFxmlWgTBLgfx0sNu9fSmnc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4569,25 +4569,25 @@
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
-          <t>yo tengo ya dos a quien en riohacha en sao venden</t>
+          <t>ya se dieron cuenta que Coca-Cola trajo nuevamente los hielocos.</t>
         </is>
       </c>
       <c r="G74" s="2" t="n">
-        <v>45928.95106481481</v>
+        <v>45928.82883101852</v>
       </c>
       <c r="H74" s="3" t="n">
         <v>45928</v>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>22:49:32</t>
+          <t>19:53:31</t>
         </is>
       </c>
       <c r="J74" t="n">
         <v>0</v>
       </c>
       <c r="K74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L74" t="b">
         <v>0</v>
@@ -4599,7 +4599,7 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555275859973767956', 'createTime': 1759099772, 'createTimeISO': '2025-09-28T22:49:32.000Z', 'text': 'yo tengo ya dos a quien en riohacha en sao venden', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7424964499378504710', 'uniqueId': 'belkis.palmezano', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/4bf65fc92b7418231543d485d5032734~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=d0d80cc6&amp;x-expires=1759593600&amp;x-signature=XYoo%2BHAwnTC6sV9dvvFc6YdE1Z8%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555230564963648264', 'createTime': 1759089211, 'createTimeISO': '2025-09-28T19:53:31.000Z', 'text': 'ya se dieron cuenta que Coca-Cola trajo nuevamente los hielocos.', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '7311721551714796549', 'uniqueId': 'junior.xd.velez', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/7311721679486386181~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=309b0e06&amp;x-expires=1760619600&amp;x-signature=eoxLw6h%2FzD2ULwnd%2BM6nzrmHGW4%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4625,18 +4625,18 @@
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
-          <t>si claro si yo vivo en colomb</t>
+          <t>si algo eso cuántos Mochis me dan</t>
         </is>
       </c>
       <c r="G75" s="2" t="n">
-        <v>45930.02231481481</v>
+        <v>45942.7344212963</v>
       </c>
       <c r="H75" s="3" t="n">
-        <v>45930</v>
+        <v>45942</v>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>00:32:08</t>
+          <t>17:37:34</t>
         </is>
       </c>
       <c r="J75" t="n">
@@ -4655,7 +4655,7 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555673462803694343', 'createTime': 1759192328, 'createTimeISO': '2025-09-30T00:32:08.000Z', 'text': 'si claro si yo vivo en colomb', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7552728943149810705', 'uniqueId': 'dannasofi6899', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/865736a245746c0e4f5e41bb7590a553~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=ec2344a9&amp;x-expires=1759593600&amp;x-signature=Xhmqj2cjeqniOn25TYus7VTN4B0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7560390745014960912', 'createTime': 1760290654, 'createTimeISO': '2025-10-12T17:37:34.000Z', 'text': 'si algo eso cuántos Mochis me dan', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7454562571774018566', 'uniqueId': 'mariposas6818', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/e9a766a7989642f5f3b2b8341519efa8~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=63413d82&amp;x-expires=1760619600&amp;x-signature=z1syxgCV%2BK9%2Fz6OUEPsvbcIFQfk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4681,18 +4681,18 @@
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr">
         <is>
-          <t>eran mejor los gogos</t>
+          <t>Yo quiero</t>
         </is>
       </c>
       <c r="G76" s="2" t="n">
-        <v>45929.47387731481</v>
+        <v>45935.77395833333</v>
       </c>
       <c r="H76" s="3" t="n">
-        <v>45929</v>
+        <v>45935</v>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>11:22:23</t>
+          <t>18:34:30</t>
         </is>
       </c>
       <c r="J76" t="n">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555469953446052609', 'createTime': 1759144943, 'createTimeISO': '2025-09-29T11:22:23.000Z', 'text': 'eran mejor los gogos', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7228579787227350022', 'uniqueId': 'diazsergio448', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-maliva-avt-0068/61df6591ddc0252c4f89c7801a873c3c~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=01f44597&amp;x-expires=1759593600&amp;x-signature=p6JMc76ZWNlw9jusuaMI6pJDIps%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7557807836890645255', 'createTime': 1759689270, 'createTimeISO': '2025-10-05T18:34:30.000Z', 'text': 'Yo quiero', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7543462359529440276', 'uniqueId': 'annie.carolina7', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/d2456170bcdac850e36cf4089df9b648~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=ed5c0cb1&amp;x-expires=1760619600&amp;x-signature=ouVG3d%2Bufr0GGoAmeWdbW9Xm0iE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4737,18 +4737,18 @@
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Ahora si lo pusieron más costosos JAAJJAA</t>
+          <t>menos mal, porque esos mini Mochis nada que ver</t>
         </is>
       </c>
       <c r="G77" s="2" t="n">
-        <v>45926.97465277778</v>
+        <v>45927.03719907408</v>
       </c>
       <c r="H77" s="3" t="n">
-        <v>45926</v>
+        <v>45927</v>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>23:23:30</t>
+          <t>00:53:34</t>
         </is>
       </c>
       <c r="J77" t="n">
@@ -4767,7 +4767,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554542515267437332', 'createTime': 1758929010, 'createTimeISO': '2025-09-26T23:23:30.000Z', 'text': 'Ahora si lo pusieron más costosos JAAJJAA', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7195421632918782981', 'uniqueId': 'catefe14', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/3b04b15a99963776fbad8b9ebe9edbe8~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=d7d0f635&amp;x-expires=1759593600&amp;x-signature=HtbYTdV3RZ5v2vSAfqaaXBB281M%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554565731141354248', 'createTime': 1758934414, 'createTimeISO': '2025-09-27T00:53:34.000Z', 'text': 'menos mal, porque esos mini Mochis nada que ver', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '306200608217440256', 'uniqueId': 'adrianacontajaram', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/3ca1721c854ebb7d5a1c458fad6e8110~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=af12a055&amp;x-expires=1760619600&amp;x-signature=Oy%2BFwE0OR78ZERf1J4%2Foexqiz84%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4793,18 +4793,18 @@
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Ahhh soy fan suyos y tengo la colección de los chicitos y los grandes y los de bolso ya los 40 😌</t>
+          <t>don hermosos</t>
         </is>
       </c>
       <c r="G78" s="2" t="n">
-        <v>45927.60967592592</v>
+        <v>45940.69850694444</v>
       </c>
       <c r="H78" s="3" t="n">
-        <v>45927</v>
+        <v>45940</v>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>14:37:56</t>
+          <t>16:45:51</t>
         </is>
       </c>
       <c r="J78" t="n">
@@ -4823,7 +4823,7 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554778199965123335', 'createTime': 1758983876, 'createTimeISO': '2025-09-27T14:37:56.000Z', 'text': 'Ahhh soy fan suyos y tengo la colección de los chicitos y los grandes y los de bolso ya los 40 😌', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7427943544844190726', 'uniqueId': 'luci_123461', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/22c7a80abcc4d081e648ea0fbef7e176~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=38abd7b9&amp;x-expires=1759593600&amp;x-signature=P4eEtNkm0XJKYkQFm%2BAOCCbx7rs%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7559635269188829959', 'createTime': 1760114751, 'createTimeISO': '2025-10-10T16:45:51.000Z', 'text': 'don hermosos', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7462015983667545094', 'uniqueId': 'yura2495', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/745aa78c04c60c9088a11c6f996f3307~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=0f023d57&amp;x-expires=1760619600&amp;x-signature=ALieX%2B0azC%2FIMyng2J4rXeJ8kzU%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4849,25 +4849,25 @@
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
-          <t>pueden quitar los mochis y volver a poner los muñequitos de gokuuuu por favor</t>
+          <t>pero si ya corte los logos y no corte lo que dice mochisaurios y tampoco tengo el código??</t>
         </is>
       </c>
       <c r="G79" s="2" t="n">
-        <v>45930.20326388889</v>
+        <v>45929.11127314815</v>
       </c>
       <c r="H79" s="3" t="n">
-        <v>45930</v>
+        <v>45929</v>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>04:52:42</t>
+          <t>02:40:14</t>
         </is>
       </c>
       <c r="J79" t="n">
         <v>0</v>
       </c>
       <c r="K79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L79" t="b">
         <v>0</v>
@@ -4879,7 +4879,7 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555740607941067527', 'createTime': 1759207962, 'createTimeISO': '2025-09-30T04:52:42.000Z', 'text': 'pueden quitar los mochis y volver a poner los muñequitos de gokuuuu por favor', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7414501088697861126', 'uniqueId': 'samu__777a_', 'avatarThumbnail': 'https://p19-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/758a25c5c7f3a69b27a4c51c3756f1f3~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=61d07ae3&amp;x-expires=1759593600&amp;x-signature=p6oH4To8jwnjmCXXEDTcwaNQ58Y%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555335413934981895', 'createTime': 1759113614, 'createTimeISO': '2025-09-29T02:40:14.000Z', 'text': 'pero si ya corte los logos y no corte lo que dice mochisaurios y tampoco tengo el código??', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 1, 'uid': '6887020420505109509', 'uniqueId': 'mari_a0131', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/52b610568365088bb8157c0e968fb5e0~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=adbdee11&amp;x-expires=1760619600&amp;x-signature=d%2FWev7ARz%2FoTxIa3Z9xy6iqXRoM%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4905,18 +4905,18 @@
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
-          <t>esta vez está más facil conseguirlos en alkosto pasto , más barato , los encuentras de varios sabores el yogo premio 🥰</t>
+          <t>amooo los mochiss</t>
         </is>
       </c>
       <c r="G80" s="2" t="n">
-        <v>45933.06369212963</v>
+        <v>45930.14606481481</v>
       </c>
       <c r="H80" s="3" t="n">
-        <v>45933</v>
+        <v>45930</v>
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>01:31:43</t>
+          <t>03:30:20</t>
         </is>
       </c>
       <c r="J80" t="n">
@@ -4935,7 +4935,7 @@
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556802057828451090', 'createTime': 1759455103, 'createTimeISO': '2025-10-03T01:31:43.000Z', 'text': 'esta vez está más facil conseguirlos en alkosto pasto , más barato , los encuentras de varios sabores el yogo premio 🥰', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6871021709530334214', 'uniqueId': 'dianajs20', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/d1b80594f31b301f5b7d2a17f8ebf07a~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=5b994380&amp;x-expires=1759593600&amp;x-signature=vL6yzocbuZ0ldwjIDISfwzWYKNY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555719396933829377', 'createTime': 1759203020, 'createTimeISO': '2025-09-30T03:30:20.000Z', 'text': 'amooo los mochiss', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7367208908349621253', 'uniqueId': 'temasammy', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/1710e3752cd7ef1d903ec79c90068b53~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=6b24fd9b&amp;x-expires=1760619600&amp;x-signature=DxSQlgjAnmocCEsE9Tf7zMrF%2BRY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -4961,18 +4961,18 @@
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Vivo al frente del Oxxo 🫦</t>
+          <t>oigan pero no encuentro mochisaurios solo ilumimochis</t>
         </is>
       </c>
       <c r="G81" s="2" t="n">
-        <v>45927.91778935185</v>
+        <v>45932.81353009259</v>
       </c>
       <c r="H81" s="3" t="n">
-        <v>45927</v>
+        <v>45932</v>
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>22:01:37</t>
+          <t>19:31:29</t>
         </is>
       </c>
       <c r="J81" t="n">
@@ -4991,7 +4991,7 @@
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554892480945357575', 'createTime': 1759010497, 'createTimeISO': '2025-09-27T22:01:37.000Z', 'text': 'Vivo al frente del Oxxo \U0001fae6', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7364587532505613318', 'uniqueId': 'its_valerytt', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/fa3a6ffbfa7cac32480206d4dfcc4155~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=dfb36516&amp;x-expires=1759593600&amp;x-signature=BK29lp5QGK4OyvI%2Bvsha%2FmFp11s%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556709242481722130', 'createTime': 1759433489, 'createTimeISO': '2025-10-02T19:31:29.000Z', 'text': 'oigan pero no encuentro mochisaurios solo ilumimochis', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7121425545787868165', 'uniqueId': 'filosofia.gatuna', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/611472f8abb9c3c4e66c407a80c4ee1b~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=5ab0f595&amp;x-expires=1760619600&amp;x-signature=PAUY2twnwg7KdYqIHYml6x0h%2FaM%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5017,18 +5017,18 @@
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr">
         <is>
-          <t>yo vivo en sincelejo</t>
+          <t>Y para cuándo los YoYos de YogoYogo !!</t>
         </is>
       </c>
       <c r="G82" s="2" t="n">
-        <v>45927.42297453704</v>
+        <v>45937.61719907408</v>
       </c>
       <c r="H82" s="3" t="n">
-        <v>45927</v>
+        <v>45937</v>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>10:09:05</t>
+          <t>14:48:46</t>
         </is>
       </c>
       <c r="J82" t="n">
@@ -5047,7 +5047,7 @@
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554708918883107605', 'createTime': 1758967745, 'createTimeISO': '2025-09-27T10:09:05.000Z', 'text': 'yo vivo en sincelejo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7528863782614778887', 'uniqueId': 'maria.del.mar609', 'avatarThumbnail': 'https://p19-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/bd1608f690c965c3486708670f3bfd79~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=4199551d&amp;x-expires=1759593600&amp;x-signature=0APgfvGPZmzxtPvr178fL29OfuU%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast8', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7558491815541441281', 'createTime': 1759848526, 'createTimeISO': '2025-10-07T14:48:46.000Z', 'text': 'Y para cuándo los YoYos de YogoYogo !!', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7464018882559804434', 'uniqueId': 'mastervelas10', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/musically-maliva-obj/1594805258216454~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=bc9f0393&amp;x-expires=1760619600&amp;x-signature=RzCGUMv6hD3iDnmfkXd8UVKMMgE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5073,18 +5073,18 @@
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Yo ese muñeco me lo encontré en el baño de la escuela y nuevo estaba</t>
+          <t>Yo y los que reclamamos todos los que tenían en la tienda porque soy una adicta al yogo yogo (porfis déjenme patrocinar o regálenme algo tengo el peluche de la máquina y todas las colecciones incompletas pero las tengo)</t>
         </is>
       </c>
       <c r="G83" s="2" t="n">
-        <v>45932.80388888889</v>
+        <v>45935.07732638889</v>
       </c>
       <c r="H83" s="3" t="n">
-        <v>45932</v>
+        <v>45935</v>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>19:17:36</t>
+          <t>01:51:21</t>
         </is>
       </c>
       <c r="J83" t="n">
@@ -5103,7 +5103,7 @@
       </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556705655765648146', 'createTime': 1759432656, 'createTimeISO': '2025-10-02T19:17:36.000Z', 'text': 'Yo ese muñeco me lo encontré en el baño de la escuela y nuevo estaba', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7510321373261202450', 'uniqueId': 'bri_p2014', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/b2e1273161d281818edc50c3450cfdcb~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=371a4451&amp;x-expires=1759593600&amp;x-signature=0vXPbdNXdTLYSCvH8EAA7F5ZuNk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7557549302736208647', 'createTime': 1759629081, 'createTimeISO': '2025-10-05T01:51:21.000Z', 'text': 'Yo y los que reclamamos todos los que tenían en la tienda porque soy una adicta al yogo yogo (porfis déjenme patrocinar o regálenme algo tengo el peluche de la máquina y todas las colecciones incompletas pero las tengo)', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6844340518231802886', 'uniqueId': 'bingobaby89newaccount', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/03318f67407fffda8cd02378e395034e~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=a3210cb1&amp;x-expires=1760619600&amp;x-signature=i7LsJoumPOVHZE49hBRByqhIVZ4%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5160,7 +5160,7 @@
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555661675728044807', 'createTime': 1759189595, 'createTimeISO': '2025-09-29T23:46:35.000Z', 'text': 'el otro año mochisauros q iluminan\nte dio hambre yogo yogo [sticker]', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7229492920381899781', 'uniqueId': 'ortiz.1400', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/de36f59531a8946d7c3c30cab3c29c87~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=16325c4f&amp;x-expires=1759593600&amp;x-signature=xclQaNOEvA9gpCdh9PAnPONQPM0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555661675728044807', 'createTime': 1759189595, 'createTimeISO': '2025-09-29T23:46:35.000Z', 'text': 'el otro año mochisauros q iluminan\nte dio hambre yogo yogo [sticker]', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7229492920381899781', 'uniqueId': 'ortiz.1400', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/de36f59531a8946d7c3c30cab3c29c87~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=22a4401a&amp;x-expires=1760619600&amp;x-signature=w1sztTSNZBo7Or0cz8r2AQe%2BL4U%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5186,18 +5186,18 @@
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Ami me salió un unicornio en uno</t>
+          <t>me encantan los mochis mi mamá nunca me compra ninguno creo que me dejes hacer ⭐😍</t>
         </is>
       </c>
       <c r="G85" s="2" t="n">
-        <v>45932.92136574074</v>
+        <v>45939.96612268518</v>
       </c>
       <c r="H85" s="3" t="n">
-        <v>45932</v>
+        <v>45939</v>
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>22:06:46</t>
+          <t>23:11:13</t>
         </is>
       </c>
       <c r="J85" t="n">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556749197270991637', 'createTime': 1759442806, 'createTimeISO': '2025-10-02T22:06:46.000Z', 'text': 'Ami me salió un unicornio en uno', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7316406165842740230', 'uniqueId': 'michirobloxfnafcolombia', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/811b5143a6b4c89721b77c47d0f3a4cf~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=acc609a4&amp;x-expires=1759593600&amp;x-signature=O%2BKAoPKZklrjLIe3FqFefDAnePE%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7559363418022249224', 'createTime': 1760051473, 'createTimeISO': '2025-10-09T23:11:13.000Z', 'text': 'me encantan los mochis mi mamá nunca me compra ninguno creo que me dejes hacer ⭐😍', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7381557792702153734', 'uniqueId': 'luchiii4155', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/25933fce4e672e9823eb77161e1bdb88~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=fd3ca8f5&amp;x-expires=1760619600&amp;x-signature=4y195K9EuU9RG7T4DlRNw3wOAFA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5242,18 +5242,18 @@
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
         <is>
-          <t>ya tengo muchooosss</t>
+          <t>esta vez está más facil conseguirlos en alkosto pasto , más barato , los encuentras de varios sabores el yogo premio 🥰</t>
         </is>
       </c>
       <c r="G86" s="2" t="n">
-        <v>45929.9649074074</v>
+        <v>45933.06369212963</v>
       </c>
       <c r="H86" s="3" t="n">
-        <v>45929</v>
+        <v>45933</v>
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>23:09:28</t>
+          <t>01:31:43</t>
         </is>
       </c>
       <c r="J86" t="n">
@@ -5272,7 +5272,7 @@
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555652136999453447', 'createTime': 1759187368, 'createTimeISO': '2025-09-29T23:09:28.000Z', 'text': 'ya tengo muchooosss', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7452352762484507654', 'uniqueId': 'glxsyy_gaby', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/f640f746bac5eb67f15e4c8ed375d287~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=fb061a4d&amp;x-expires=1759593600&amp;x-signature=oOisdud%2FMniOIfDStW13xgDC10o%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556802057828451090', 'createTime': 1759455103, 'createTimeISO': '2025-10-03T01:31:43.000Z', 'text': 'esta vez está más facil conseguirlos en alkosto pasto , más barato , los encuentras de varios sabores el yogo premio 🥰', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6871021709530334214', 'uniqueId': 'dianajs20', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/d1b80594f31b301f5b7d2a17f8ebf07a~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=54658a86&amp;x-expires=1760619600&amp;x-signature=XKAlh%2BLgUs6ZAyg%2Fdu3IqRBibEo%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5298,18 +5298,18 @@
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
-          <t>GRQCIASS. ME DIOO UNOO😭💜</t>
+          <t>ya no es lo mismo</t>
         </is>
       </c>
       <c r="G87" s="2" t="n">
-        <v>45927.89190972222</v>
+        <v>45940.20726851852</v>
       </c>
       <c r="H87" s="3" t="n">
-        <v>45927</v>
+        <v>45940</v>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>21:24:21</t>
+          <t>04:58:28</t>
         </is>
       </c>
       <c r="J87" t="n">
@@ -5328,7 +5328,7 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554882846906811137', 'createTime': 1759008261, 'createTimeISO': '2025-09-27T21:24:21.000Z', 'text': 'GRQCIASS. ME DIOO UNOO😭💜', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7306695570843550725', 'uniqueId': 'astro_shelly5', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/a97d6db6bc7fbe92e2a5c87ec99db37b~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=c66246d1&amp;x-expires=1759593600&amp;x-signature=PM0EfFI4pgYiBP%2BQYfLZD%2Ft9DC8%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7559452964297917200', 'createTime': 1760072308, 'createTimeISO': '2025-10-10T04:58:28.000Z', 'text': 'ya no es lo mismo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7440309516846367800', 'uniqueId': 'user3866547831001', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/c5d23423bddcf59c497bd0d1bdeea6ad~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=7b87d8c0&amp;x-expires=1760619600&amp;x-signature=nuKVlZmlGCVaT2H8QToUmWkfp14%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5354,18 +5354,18 @@
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr">
         <is>
-          <t>y si estoy en Colombia</t>
+          <t>ami me sale pura cagada un día me salió un unicornio y hoy me salió un cocodrilo (T_T)</t>
         </is>
       </c>
       <c r="G88" s="2" t="n">
-        <v>45930.03666666667</v>
+        <v>45935.94721064815</v>
       </c>
       <c r="H88" s="3" t="n">
-        <v>45930</v>
+        <v>45935</v>
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>00:52:48</t>
+          <t>22:43:59</t>
         </is>
       </c>
       <c r="J88" t="n">
@@ -5384,7 +5384,7 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555678757781422856', 'createTime': 1759193568, 'createTimeISO': '2025-09-30T00:52:48.000Z', 'text': 'y si estoy en Colombia', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7511370345698526228', 'uniqueId': 'eslendy121', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/17b0bce09c224ef4b7b58274a200d715~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=356c618a&amp;x-expires=1759593600&amp;x-signature=N%2Fsjeh8JSyb7XjWBdDt3rzX5AVc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7557872085788656392', 'createTime': 1759704239, 'createTimeISO': '2025-10-05T22:43:59.000Z', 'text': '𝚊𝚖𝚒 𝚖𝚎 𝚜𝚊𝚕𝚎 𝚙𝚞𝚛𝚊 𝚌𝚊𝚐𝚊𝚍𝚊 𝚞𝚗 𝚍𝚒́𝚊 𝚖𝚎 𝚜𝚊𝚕𝚒𝚘́ 𝚞𝚗 𝚞𝚗𝚒𝚌𝚘𝚛𝚗𝚒𝚘 𝚢 𝚑𝚘𝚢 𝚖𝚎 𝚜𝚊𝚕𝚒𝚘́ 𝚞𝚗 𝚌𝚘𝚌𝚘𝚍𝚛𝚒𝚕𝚘 (T_T)', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7398980026529760262', 'uniqueId': 'salome.murcia.lop', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/340cd1e87c2a55967180747c200950a3~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=3c85bbd0&amp;x-expires=1760619600&amp;x-signature=BwbCSl%2BpLOyXsvA%2FBctToxmyObk%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5410,18 +5410,18 @@
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Excelente. Hacen falta estas promociones en los productos y que mejoren la calidad de la leche en bolsa</t>
+          <t>Ami me salió un unicornio en uno</t>
         </is>
       </c>
       <c r="G89" s="2" t="n">
-        <v>45929.1794212963</v>
+        <v>45932.92136574074</v>
       </c>
       <c r="H89" s="3" t="n">
-        <v>45929</v>
+        <v>45932</v>
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>04:18:22</t>
+          <t>22:06:46</t>
         </is>
       </c>
       <c r="J89" t="n">
@@ -5440,7 +5440,7 @@
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555360657135682321', 'createTime': 1759119502, 'createTimeISO': '2025-09-29T04:18:22.000Z', 'text': 'Excelente. Hacen falta estas promociones en los productos y que mejoren la calidad de la leche en bolsa', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6816660881625465862', 'uniqueId': 'gatusso88.88', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/d08015a0ec17b31fabb0d96423b6fbd1~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=2b66b5ce&amp;x-expires=1759593600&amp;x-signature=JAxucPECS2ZXLGzh0owPgL8vdTY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556749197270991637', 'createTime': 1759442806, 'createTimeISO': '2025-10-02T22:06:46.000Z', 'text': 'Ami me salió un unicornio en uno', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7316406165842740230', 'uniqueId': 'michirobloxfnafcolombia', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/811b5143a6b4c89721b77c47d0f3a4cf~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=b8cdaff5&amp;x-expires=1760619600&amp;x-signature=3bCL0Ha2kVVD5N3RWsiQXX%2Buee0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5466,18 +5466,18 @@
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr">
         <is>
-          <t>por favor vuelve a los muñequitos de antes ya no quiero más mochis</t>
+          <t>y para que sirve eso, que beneficios tiene 😳</t>
         </is>
       </c>
       <c r="G90" s="2" t="n">
-        <v>45929.88721064815</v>
+        <v>45933.05707175926</v>
       </c>
       <c r="H90" s="3" t="n">
-        <v>45929</v>
+        <v>45933</v>
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>21:17:35</t>
+          <t>01:22:11</t>
         </is>
       </c>
       <c r="J90" t="n">
@@ -5496,7 +5496,7 @@
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555623204544824080', 'createTime': 1759180655, 'createTimeISO': '2025-09-29T21:17:35.000Z', 'text': 'por favor vuelve a los muñequitos de antes ya no quiero más mochis', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7181553216034079750', 'uniqueId': 'emanuelmeza1976', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/c6ce45f84f08573022367e687a3e5e79~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=df2d9025&amp;x-expires=1759593600&amp;x-signature=EcQfrfP5rXMnw3eEz4k5jUvit4Y%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556799608577458951', 'createTime': 1759454531, 'createTimeISO': '2025-10-03T01:22:11.000Z', 'text': 'y para que sirve eso, que beneficios tiene 😳', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6935601595720860678', 'uniqueId': 'monica_lenis1980', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/fce7942c402b7371d210f51cf61e58d9~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=a50d12db&amp;x-expires=1760619600&amp;x-signature=MCcb9ozEueitSEvOcSoZ6YQGMNU%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5522,18 +5522,18 @@
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr">
         <is>
-          <t>yo soy de pitalito huila y no hay oxxo</t>
+          <t>no hay plata 💔</t>
         </is>
       </c>
       <c r="G91" s="2" t="n">
-        <v>45928.77608796296</v>
+        <v>45943.12447916667</v>
       </c>
       <c r="H91" s="3" t="n">
-        <v>45928</v>
+        <v>45943</v>
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>18:37:34</t>
+          <t>02:59:15</t>
         </is>
       </c>
       <c r="J91" t="n">
@@ -5552,7 +5552,7 @@
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555211031862461191', 'createTime': 1759084654, 'createTimeISO': '2025-09-28T18:37:34.000Z', 'text': 'yo soy de pitalito huila y no hay oxxo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7271470368271188998', 'uniqueId': 'luisferneysilvago', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/7360438781521821701~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=95dbe266&amp;x-expires=1759593600&amp;x-signature=lIoyASAo9G2Ylqt8Ia6nbDREumA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7560535489130300168', 'createTime': 1760324355, 'createTimeISO': '2025-10-13T02:59:15.000Z', 'text': 'no hay plata 💔', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7455861170257249300', 'uniqueId': 'eminemxd19', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/81a571f9081a325ea0b63e6179cc5948~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=ebb5d862&amp;x-expires=1760619600&amp;x-signature=Nz16ZTZe8CO0LyNDQ3JJRxRXjQM%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5578,18 +5578,18 @@
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr">
         <is>
-          <t>pero sola mente sonos logos que disen todo yogo</t>
+          <t>pensándolo bien se ven hermosos 😻💗</t>
         </is>
       </c>
       <c r="G92" s="2" t="n">
-        <v>45930.0090162037</v>
+        <v>45940.70783564815</v>
       </c>
       <c r="H92" s="3" t="n">
-        <v>45930</v>
+        <v>45940</v>
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>00:12:59</t>
+          <t>16:59:17</t>
         </is>
       </c>
       <c r="J92" t="n">
@@ -5608,7 +5608,7 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555668487608582928', 'createTime': 1759191179, 'createTimeISO': '2025-09-30T00:12:59.000Z', 'text': 'pero sola mente sonos logos que disen todo yogo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7352935562129802246', 'uniqueId': 'titta4841', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/musically-maliva-obj/1594805258216454~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=181da6bc&amp;x-expires=1759593600&amp;x-signature=eHva4112j2iAr0GG0X%2F2bTiXJFA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7559638710619226881', 'createTime': 1760115557, 'createTimeISO': '2025-10-10T16:59:17.000Z', 'text': 'pensándolo bien se ven hermosos 😻💗', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6893194958128972801', 'uniqueId': 'nicollesofiaram98', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/66383e9c8e505f28006c4cbf3c42e837~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=9d26c530&amp;x-expires=1760619600&amp;x-signature=FERpRMa76c5wHXOsluY%2FrRvXwh4%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5634,18 +5634,18 @@
       <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr">
         <is>
-          <t>alguien sabe si aceptan los mismos paquetes de los yogopremio? 🥹 los logos</t>
+          <t>alpinaa eres el mejor me gustan tus productos❤</t>
         </is>
       </c>
       <c r="G93" s="2" t="n">
-        <v>45928.79943287037</v>
+        <v>45939.82650462963</v>
       </c>
       <c r="H93" s="3" t="n">
-        <v>45928</v>
+        <v>45939</v>
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>19:11:11</t>
+          <t>19:50:10</t>
         </is>
       </c>
       <c r="J93" t="n">
@@ -5664,7 +5664,7 @@
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555219507196871441', 'createTime': 1759086671, 'createTimeISO': '2025-09-28T19:11:11.000Z', 'text': 'alguien sabe si aceptan los mismos paquetes de los yogopremio? \U0001f979 los logos', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7248270860224578565', 'uniqueId': 'bangchanmegustas', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/93a2007f320c35921254108bfb01e853~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=ea669c34&amp;x-expires=1759593600&amp;x-signature=rDfOQky0JOQrXbrZ%2BScYr45EyX0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7559311644069757697', 'createTime': 1760039410, 'createTimeISO': '2025-10-09T19:50:10.000Z', 'text': 'alpinaa eres el mejor me gustan tus productos❤', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7066510018199585798', 'uniqueId': 'dianalozanomorera', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/95486b2edc8f09f2d015ae33f705fe3f~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=00e6f386&amp;x-expires=1760619600&amp;x-signature=fJnB93V9fVBb6JeE8zFDMMP0JgM%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5690,18 +5690,18 @@
       <c r="E94" t="inlineStr"/>
       <c r="F94" t="inlineStr">
         <is>
-          <t>nesecitoo la lista de los cuarenta muchis y nombrees</t>
+          <t>tengo 14 en total ajaja</t>
         </is>
       </c>
       <c r="G94" s="2" t="n">
-        <v>45929.73436342592</v>
+        <v>45938.74841435185</v>
       </c>
       <c r="H94" s="3" t="n">
-        <v>45929</v>
+        <v>45938</v>
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>17:37:29</t>
+          <t>17:57:43</t>
         </is>
       </c>
       <c r="J94" t="n">
@@ -5720,7 +5720,7 @@
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555566632794702599', 'createTime': 1759167449, 'createTimeISO': '2025-09-29T17:37:29.000Z', 'text': 'nesecitoo la lista de los cuarenta muchis y nombrees', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7476832145886741524', 'uniqueId': 'eli491676', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/de51a904dddc57525965d4639f48e5d4~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=e9feb323&amp;x-expires=1759593600&amp;x-signature=U6%2FohNNYCFEgU7%2FTmLb%2BLKX6yuw%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7558911601061217032', 'createTime': 1759946263, 'createTimeISO': '2025-10-08T17:57:43.000Z', 'text': 'tengo 14 en total ajaja', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7290284449584514053', 'uniqueId': 'not.dnaa', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/c359f92f7ed83771ef9e0d8b18401862~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=d6a4f570&amp;x-expires=1760619600&amp;x-signature=dDY8L8kOw4vvJtIeJ7qpcwCaD4U%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5746,18 +5746,18 @@
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr">
         <is>
-          <t>en mi ciudad no hay OXXO 😭😭😭😭😭😭</t>
+          <t>YO LLEVO SOLO 10 😭😭🗣️🗣</t>
         </is>
       </c>
       <c r="G95" s="2" t="n">
-        <v>45931.94755787037</v>
+        <v>45945.12975694444</v>
       </c>
       <c r="H95" s="3" t="n">
-        <v>45931</v>
+        <v>45945</v>
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>22:44:29</t>
+          <t>03:06:51</t>
         </is>
       </c>
       <c r="J95" t="n">
@@ -5776,7 +5776,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7556387852227035922', 'createTime': 1759358669, 'createTimeISO': '2025-10-01T22:44:29.000Z', 'text': 'en mi ciudad no hay OXXO 😭😭😭😭😭😭', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7489833937218028562', 'uniqueId': 'alexa28070', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/e12e85635aa01b27ccab64c2b8145234~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=e6cbc643&amp;x-expires=1759593600&amp;x-signature=rPdVy06xoTfswFabRcSokXrbmaY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7561279629291111176', 'createTime': 1760497611, 'createTimeISO': '2025-10-15T03:06:51.000Z', 'text': 'YO LLEVO SOLO 10 😭😭🗣️🗣', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7500744921117230081', 'uniqueId': 'l0veworld0', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/4de1e833be3b97b2d4fdf7b32557b65a~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=1b97e13b&amp;x-expires=1760619600&amp;x-signature=Y11zl8eQKH0JR7znvHii6Qae03c%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5802,18 +5802,18 @@
       <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr">
         <is>
-          <t>acá no hay oxo 😔🙃</t>
+          <t>Alpina me salió el t-rex morado pero me salió rojo</t>
         </is>
       </c>
       <c r="G96" s="2" t="n">
-        <v>45927.77946759259</v>
+        <v>45944.32868055555</v>
       </c>
       <c r="H96" s="3" t="n">
-        <v>45927</v>
+        <v>45944</v>
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>18:42:26</t>
+          <t>07:53:18</t>
         </is>
       </c>
       <c r="J96" t="n">
@@ -5832,7 +5832,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554841186369929992', 'createTime': 1758998546, 'createTimeISO': '2025-09-27T18:42:26.000Z', 'text': 'acá no hay oxo 😔🙃', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7507809562712376327', 'uniqueId': 'isa_9714', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/45a4b910e03b88ae6bca9622a5dfb0f0~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=50d50f39&amp;x-expires=1759593600&amp;x-signature=SXui3QmWQjnPIIYFpk%2BiFAJQTco%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7560982374209880840', 'createTime': 1760428398, 'createTimeISO': '2025-10-14T07:53:18.000Z', 'text': 'Alpina me salió el t-rex morado pero me salió rojo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7550916854894576647', 'uniqueId': 'matis.leon3', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/5ea667be5045cfb8a1ae14f867516de8~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=5d0fd8f4&amp;x-expires=1760619600&amp;x-signature=k%2Fh5KqQXq4Po6GPMDIUeYapggOU%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5858,18 +5858,18 @@
       <c r="E97" t="inlineStr"/>
       <c r="F97" t="inlineStr">
         <is>
-          <t>menos mal, porque esos mini Mochis nada que ver</t>
+          <t>4!? me e comprado 3 y no me sabía está :(</t>
         </is>
       </c>
       <c r="G97" s="2" t="n">
-        <v>45927.03719907408</v>
+        <v>45941.94193287037</v>
       </c>
       <c r="H97" s="3" t="n">
-        <v>45927</v>
+        <v>45941</v>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>00:53:34</t>
+          <t>22:36:23</t>
         </is>
       </c>
       <c r="J97" t="n">
@@ -5888,7 +5888,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554565731141354248', 'createTime': 1758934414, 'createTimeISO': '2025-09-27T00:53:34.000Z', 'text': 'menos mal, porque esos mini Mochis nada que ver', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '306200608217440256', 'uniqueId': 'adrianacontajaram', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/3ca1721c854ebb7d5a1c458fad6e8110~tplv-tiktokx-cropcenter:100:100.jpg?dr=10399&amp;refresh_token=dcc8c445&amp;x-expires=1759593600&amp;x-signature=bb8AA8iPMEd8FkY0zYcSGNTMdEw%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=no1a', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7560096565530116881', 'createTime': 1760222183, 'createTimeISO': '2025-10-11T22:36:23.000Z', 'text': '4!? me e comprado 3 y no me sabía está :(', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7406050480903095302', 'uniqueId': 'baraka8861', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/3578f8d9ee7e8e3faedd8e33c2df1a1d~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=d7b66de7&amp;x-expires=1760619600&amp;x-signature=MhKloIg1%2Fzdf%2BWCnQrVgeL0lSL4%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5914,18 +5914,18 @@
       <c r="E98" t="inlineStr"/>
       <c r="F98" t="inlineStr">
         <is>
-          <t>mi hijo tiene muchos ya</t>
+          <t>Mi hija estaba muy comprometida haciendo la recolección de logos recortados de YogoYogo los llevamos a OXXO y le dijeron que los recortó mal y no le dieron premio. Terrible me parece 0 estrellitas no vale la pena.</t>
         </is>
       </c>
       <c r="G98" s="2" t="n">
-        <v>45928.71826388889</v>
+        <v>45939.57203703704</v>
       </c>
       <c r="H98" s="3" t="n">
-        <v>45928</v>
+        <v>45939</v>
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>17:14:18</t>
+          <t>13:43:44</t>
         </is>
       </c>
       <c r="J98" t="n">
@@ -5944,7 +5944,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555189568158171922', 'createTime': 1759079658, 'createTimeISO': '2025-09-28T17:14:18.000Z', 'text': 'mi hijo tiene muchos ya', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7198591704680023046', 'uniqueId': 'lpez.amarfy', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/94bc9caafe217bbfd6ce01b82c1f3779~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=ed9692ca&amp;x-expires=1759593600&amp;x-signature=x3EIXsUTCWaCr69vc1hZS9dxiQA%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7559217240907399952', 'createTime': 1760017424, 'createTimeISO': '2025-10-09T13:43:44.000Z', 'text': 'Mi hija estaba muy comprometida haciendo la recolección de logos recortados de YogoYogo los llevamos a OXXO y le dijeron que los recortó mal y no le dieron premio. Terrible me parece 0 estrellitas no vale la pena.', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6790690337766556677', 'uniqueId': 'natyzhurra8', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/2ec67cba7b200e2c6b2709b67daa84b1~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=77e91b13&amp;x-expires=1760619600&amp;x-signature=KcSwtxjJ11Q1Wc%2BMWx7hpF%2BEsm8%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -5970,18 +5970,18 @@
       <c r="E99" t="inlineStr"/>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Instagram de la chica?</t>
+          <t>sale más fácil comprarles el yogo premio ahí vienen esos muñecos👌</t>
         </is>
       </c>
       <c r="G99" s="2" t="n">
-        <v>45929.91350694445</v>
+        <v>45937.1734375</v>
       </c>
       <c r="H99" s="3" t="n">
-        <v>45929</v>
+        <v>45937</v>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>21:55:27</t>
+          <t>04:09:45</t>
         </is>
       </c>
       <c r="J99" t="n">
@@ -6000,7 +6000,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555633048105779986', 'createTime': 1759182927, 'createTimeISO': '2025-09-29T21:55:27.000Z', 'text': 'Instagram de la chica?', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6918025814152201222', 'uniqueId': 'erick_armando.3', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/754d99b04476871c7f12cbaf0d1f1743~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=224569d0&amp;x-expires=1759593600&amp;x-signature=C%2FiRH7eA5X10yu0jMSILVjG0dJc%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7558327143747928848', 'createTime': 1759810185, 'createTimeISO': '2025-10-07T04:09:45.000Z', 'text': 'sale más fácil comprarles el yogo premio ahí vienen esos muñecos👌', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7270238153704342533', 'uniqueId': 'paola.rodriguez228', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/17617c83aeaf41558f9b9b48472d32af~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=0a20a60f&amp;x-expires=1760619600&amp;x-signature=sZsYu0LwLR7UBoRx7KkiMEbzwDM%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -6026,18 +6026,18 @@
       <c r="E100" t="inlineStr"/>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Amooo</t>
+          <t>loooos amooooooo❤️❤️❤️❤️❤</t>
         </is>
       </c>
       <c r="G100" s="2" t="n">
-        <v>45928.79438657407</v>
+        <v>45936.85996527778</v>
       </c>
       <c r="H100" s="3" t="n">
-        <v>45928</v>
+        <v>45936</v>
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>19:03:55</t>
+          <t>20:38:21</t>
         </is>
       </c>
       <c r="J100" t="n">
@@ -6056,7 +6056,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7555217811128615687', 'createTime': 1759086235, 'createTimeISO': '2025-09-28T19:03:55.000Z', 'text': 'Amooo', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7284419691349607430', 'uniqueId': 'kdruiz22', 'avatarThumbnail': 'https://p16-sign-va.tiktokcdn.com/tos-maliva-avt-0068/7300345897722839046~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=7fa1de1c&amp;x-expires=1759593600&amp;x-signature=shKaVC0CcxKTOqt4ZF%2F%2B2jOauq8%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7558210750176805633', 'createTime': 1759783101, 'createTimeISO': '2025-10-06T20:38:21.000Z', 'text': 'loooos amooooooo❤️❤️❤️❤️❤', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7367208908349621253', 'uniqueId': 'temasammy', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/1710e3752cd7ef1d903ec79c90068b53~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=6b24fd9b&amp;x-expires=1760619600&amp;x-signature=DxSQlgjAnmocCEsE9Tf7zMrF%2BRY%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -6082,18 +6082,18 @@
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr">
         <is>
-          <t>mi mala suerte, tenía dos abri un yogurt y me salió repetido</t>
+          <t>Hola alpina yo tengo 16 mochi saurio soy su fan</t>
         </is>
       </c>
       <c r="G101" s="2" t="n">
-        <v>45928.00234953704</v>
+        <v>45940.97159722223</v>
       </c>
       <c r="H101" s="3" t="n">
-        <v>45928</v>
+        <v>45940</v>
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>00:03:23</t>
+          <t>23:19:06</t>
         </is>
       </c>
       <c r="J101" t="n">
@@ -6112,7 +6112,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7554923850959422215', 'createTime': 1759017803, 'createTimeISO': '2025-09-28T00:03:23.000Z', 'text': 'mi mala suerte, tenía dos abri un yogurt y me salió repetido', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '7540478701881164818', 'uniqueId': 'cib_1252', 'avatarThumbnail': 'https://p16-sign-sg.tiktokcdn.com/tos-alisg-avt-0068/72330b8c5396a956cc18b2d6d1f243e7~tplv-tiktokx-cropcenter:100:100.jpg?dr=14579&amp;refresh_token=008625f1&amp;x-expires=1759593600&amp;x-signature=PC8ymdMs5nTkfSvYEuIWJcQ%2Bx5k%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=maliva', 'mentions': [], 'detailedMentions': []}</t>
+          <t>{'videoWebUrl': 'https://www.tiktok.com/@alpinacol/video/7554409105977330965', 'submittedVideoUrl': 'https://vt.tiktok.com/ZSU1kKQGb/', 'input': 'https://vt.tiktok.com/ZSU1kKQGb/', 'cid': '7559736550297633544', 'createTime': 1760138346, 'createTimeISO': '2025-10-10T23:19:06.000Z', 'text': 'Hola alpina yo tengo 16 mochi saurio soy su fan', 'diggCount': 0, 'likedByAuthor': False, 'pinnedByAuthor': False, 'repliesToId': None, 'replyCommentTotal': 0, 'uid': '6999062538463003654', 'uniqueId': 'viky34566', 'avatarThumbnail': 'https://p16-common-sign.tiktokcdn-us.com/tos-alisg-avt-0068/71919924a1b2f86ffc0e2a1190eabfbc~tplv-tiktokx-cropcenter:100:100.jpg?dr=9640&amp;refresh_token=f6134e92&amp;x-expires=1760619600&amp;x-signature=Uh%2Bs9FtGSla0r6A5NePEaPwdgO0%3D&amp;t=4d5b0474&amp;ps=13740610&amp;shp=30310797&amp;shcp=ff37627b&amp;idc=useast5', 'mentions': [], 'detailedMentions': []}</t>
         </is>
       </c>
     </row>
@@ -6180,7 +6180,7 @@
         <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>449</v>
+        <v>724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>